<commit_message>
Code Mappings, Final Compilation
</commit_message>
<xml_diff>
--- a/data/exampledata.xlsx
+++ b/data/exampledata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xbrjos\Desktop\Python\EPA-DataWorkflow\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xbrjos\Desktop\Python\DomeXLSConverter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="672" yWindow="408" windowWidth="14052" windowHeight="6036" activeTab="1"/>
+    <workbookView xWindow="672" yWindow="408" windowWidth="14052" windowHeight="6036" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="P1 info" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="818">
   <si>
     <t>BLEPA5</t>
   </si>
@@ -3997,7 +3997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -9624,10 +9624,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y134"/>
+  <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="H122" sqref="H122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9635,7 +9635,7 @@
     <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>255</v>
       </c>
@@ -9691,28 +9691,25 @@
         <v>272</v>
       </c>
       <c r="S1" s="48" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="T1" s="48" t="s">
-        <v>274</v>
-      </c>
-      <c r="U1" s="48" t="s">
         <v>275</v>
       </c>
+      <c r="U1" s="49" t="s">
+        <v>276</v>
+      </c>
       <c r="V1" s="49" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="W1" s="49" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="X1" s="49" t="s">
-        <v>278</v>
-      </c>
-      <c r="Y1" s="49" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>431</v>
       </c>
@@ -9761,25 +9758,24 @@
       </c>
       <c r="Q2" s="45"/>
       <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36" t="s">
+      <c r="S2" s="36" t="s">
         <v>433</v>
       </c>
-      <c r="U2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="32">
+        <v>33.406999999999996</v>
+      </c>
       <c r="V2" s="32">
-        <v>33.406999999999996</v>
+        <v>317</v>
       </c>
       <c r="W2" s="32">
-        <v>317</v>
+        <v>1698</v>
       </c>
       <c r="X2" s="32">
-        <v>1698</v>
-      </c>
-      <c r="Y2" s="32">
         <v>40.823</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>434</v>
       </c>
@@ -9830,25 +9826,24 @@
       <c r="R3" s="36" t="s">
         <v>435</v>
       </c>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36" t="s">
+      <c r="S3" s="36" t="s">
         <v>436</v>
       </c>
-      <c r="U3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32">
+        <v>6.1959999999999997</v>
+      </c>
       <c r="V3" s="32">
-        <v>6.1959999999999997</v>
+        <v>541</v>
       </c>
       <c r="W3" s="32">
-        <v>541</v>
+        <v>1132</v>
       </c>
       <c r="X3" s="32">
-        <v>1132</v>
-      </c>
-      <c r="Y3" s="32">
         <v>15.686</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>437</v>
       </c>
@@ -9897,25 +9892,24 @@
       </c>
       <c r="Q4" s="45"/>
       <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36" t="s">
+      <c r="S4" s="36" t="s">
         <v>438</v>
       </c>
-      <c r="U4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32">
+        <v>142.18100000000001</v>
+      </c>
       <c r="V4" s="32">
-        <v>142.18100000000001</v>
+        <v>426</v>
       </c>
       <c r="W4" s="32">
-        <v>426</v>
+        <v>498</v>
       </c>
       <c r="X4" s="32">
-        <v>498</v>
-      </c>
-      <c r="Y4" s="32">
         <v>149.011</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>439</v>
       </c>
@@ -9964,25 +9958,24 @@
       </c>
       <c r="Q5" s="45"/>
       <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="36" t="s">
+      <c r="S5" s="36" t="s">
         <v>441</v>
       </c>
-      <c r="U5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32">
+        <v>10.131</v>
+      </c>
       <c r="V5" s="32">
-        <v>10.131</v>
+        <v>362</v>
       </c>
       <c r="W5" s="32">
-        <v>362</v>
+        <v>1244</v>
       </c>
       <c r="X5" s="32">
-        <v>1244</v>
-      </c>
-      <c r="Y5" s="32">
         <v>19.992999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>442</v>
       </c>
@@ -10031,25 +10024,24 @@
       </c>
       <c r="Q6" s="45"/>
       <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36" t="s">
+      <c r="S6" s="36" t="s">
         <v>444</v>
       </c>
-      <c r="U6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32">
+        <v>89.227999999999994</v>
+      </c>
       <c r="V6" s="32">
-        <v>89.227999999999994</v>
+        <v>1103</v>
       </c>
       <c r="W6" s="32">
-        <v>1103</v>
+        <v>1786</v>
       </c>
       <c r="X6" s="32">
-        <v>1786</v>
-      </c>
-      <c r="Y6" s="32">
         <v>86.888000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>445</v>
       </c>
@@ -10098,25 +10090,24 @@
       </c>
       <c r="Q7" s="45"/>
       <c r="R7" s="36"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="36" t="s">
+      <c r="S7" s="36" t="s">
         <v>446</v>
       </c>
-      <c r="U7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="32">
+        <v>19.934999999999999</v>
+      </c>
       <c r="V7" s="32">
-        <v>19.934999999999999</v>
+        <v>275</v>
       </c>
       <c r="W7" s="32">
-        <v>275</v>
+        <v>1567</v>
       </c>
       <c r="X7" s="32">
-        <v>1567</v>
-      </c>
-      <c r="Y7" s="32">
         <v>40.052999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>447</v>
       </c>
@@ -10165,25 +10156,24 @@
       </c>
       <c r="Q8" s="45"/>
       <c r="R8" s="36"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="36" t="s">
+      <c r="S8" s="36" t="s">
         <v>448</v>
       </c>
-      <c r="U8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="32">
+        <v>147.86199999999999</v>
+      </c>
       <c r="V8" s="32">
-        <v>147.86199999999999</v>
+        <v>405</v>
       </c>
       <c r="W8" s="32">
-        <v>405</v>
+        <v>1944</v>
       </c>
       <c r="X8" s="32">
-        <v>1944</v>
-      </c>
-      <c r="Y8" s="32">
         <v>37.515000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>449</v>
       </c>
@@ -10232,25 +10222,24 @@
       </c>
       <c r="Q9" s="45"/>
       <c r="R9" s="36"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36" t="s">
+      <c r="S9" s="36" t="s">
         <v>451</v>
       </c>
-      <c r="U9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="32">
+        <v>1.5580000000000001</v>
+      </c>
       <c r="V9" s="32">
-        <v>1.5580000000000001</v>
+        <v>436</v>
       </c>
       <c r="W9" s="32">
-        <v>436</v>
+        <v>496</v>
       </c>
       <c r="X9" s="32">
-        <v>496</v>
-      </c>
-      <c r="Y9" s="32">
         <v>163.47300000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>452</v>
       </c>
@@ -10299,25 +10288,24 @@
       </c>
       <c r="Q10" s="45"/>
       <c r="R10" s="36"/>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36" t="s">
+      <c r="S10" s="36" t="s">
         <v>453</v>
       </c>
-      <c r="U10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="32">
+        <v>178.56100000000001</v>
+      </c>
       <c r="V10" s="32">
-        <v>178.56100000000001</v>
+        <v>414</v>
       </c>
       <c r="W10" s="32">
-        <v>414</v>
+        <v>975</v>
       </c>
       <c r="X10" s="32">
-        <v>975</v>
-      </c>
-      <c r="Y10" s="32">
         <v>8.3360000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>454</v>
       </c>
@@ -10366,25 +10354,24 @@
       </c>
       <c r="Q11" s="45"/>
       <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
-      <c r="T11" s="36" t="s">
+      <c r="S11" s="36" t="s">
         <v>456</v>
       </c>
-      <c r="U11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="32">
+        <v>169.62100000000001</v>
+      </c>
       <c r="V11" s="32">
-        <v>169.62100000000001</v>
+        <v>278</v>
       </c>
       <c r="W11" s="32">
-        <v>278</v>
+        <v>494</v>
       </c>
       <c r="X11" s="32">
-        <v>494</v>
-      </c>
-      <c r="Y11" s="32">
         <v>158.81899999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>457</v>
       </c>
@@ -10433,25 +10420,24 @@
       </c>
       <c r="Q12" s="45"/>
       <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36" t="s">
+      <c r="S12" s="36" t="s">
         <v>458</v>
       </c>
-      <c r="U12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="32">
+        <v>168.83799999999999</v>
+      </c>
       <c r="V12" s="32">
-        <v>168.83799999999999</v>
+        <v>324</v>
       </c>
       <c r="W12" s="32">
-        <v>324</v>
+        <v>702</v>
       </c>
       <c r="X12" s="32">
-        <v>702</v>
-      </c>
-      <c r="Y12" s="32">
         <v>155.142</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>459</v>
       </c>
@@ -10496,25 +10482,24 @@
       </c>
       <c r="Q13" s="45"/>
       <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36" t="s">
+      <c r="S13" s="36" t="s">
         <v>460</v>
       </c>
-      <c r="U13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="32">
+        <v>38.622999999999998</v>
+      </c>
       <c r="V13" s="32">
-        <v>38.622999999999998</v>
+        <v>557</v>
       </c>
       <c r="W13" s="32">
-        <v>557</v>
+        <v>1510</v>
       </c>
       <c r="X13" s="32">
-        <v>1510</v>
-      </c>
-      <c r="Y13" s="32">
         <v>23.134</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
         <v>461</v>
       </c>
@@ -10563,25 +10548,24 @@
       </c>
       <c r="Q14" s="45"/>
       <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="36" t="s">
+      <c r="S14" s="36" t="s">
         <v>462</v>
       </c>
-      <c r="U14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="32">
+        <v>166.51300000000001</v>
+      </c>
       <c r="V14" s="32">
-        <v>166.51300000000001</v>
+        <v>161</v>
       </c>
       <c r="W14" s="32">
-        <v>161</v>
+        <v>435</v>
       </c>
       <c r="X14" s="32">
-        <v>435</v>
-      </c>
-      <c r="Y14" s="32">
         <v>151.59399999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
         <v>463</v>
       </c>
@@ -10630,25 +10614,24 @@
       </c>
       <c r="Q15" s="45"/>
       <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36" t="s">
+      <c r="S15" s="36" t="s">
         <v>464</v>
       </c>
-      <c r="U15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="32">
+        <v>0.75800000000000001</v>
+      </c>
       <c r="V15" s="32">
-        <v>0.75800000000000001</v>
+        <v>297</v>
       </c>
       <c r="W15" s="32">
-        <v>297</v>
+        <v>1218</v>
       </c>
       <c r="X15" s="32">
-        <v>1218</v>
-      </c>
-      <c r="Y15" s="32">
         <v>11.004</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
         <v>465</v>
       </c>
@@ -10693,25 +10676,24 @@
       </c>
       <c r="Q16" s="45"/>
       <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36" t="s">
+      <c r="S16" s="36" t="s">
         <v>466</v>
       </c>
-      <c r="U16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="32">
+        <v>0.66300000000000003</v>
+      </c>
       <c r="V16" s="32">
-        <v>0.66300000000000003</v>
+        <v>262</v>
       </c>
       <c r="W16" s="32">
-        <v>262</v>
+        <v>1052</v>
       </c>
       <c r="X16" s="32">
-        <v>1052</v>
-      </c>
-      <c r="Y16" s="32">
         <v>7.9210000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="36" t="s">
         <v>467</v>
       </c>
@@ -10760,25 +10742,24 @@
       </c>
       <c r="Q17" s="45"/>
       <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36" t="s">
+      <c r="S17" s="36" t="s">
         <v>468</v>
       </c>
-      <c r="U17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="32">
+        <v>3.302</v>
+      </c>
       <c r="V17" s="32">
-        <v>3.302</v>
+        <v>259</v>
       </c>
       <c r="W17" s="32">
-        <v>259</v>
+        <v>1204</v>
       </c>
       <c r="X17" s="32">
-        <v>1204</v>
-      </c>
-      <c r="Y17" s="32">
         <v>8.0009999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="36" t="s">
         <v>469</v>
       </c>
@@ -10827,25 +10808,24 @@
       </c>
       <c r="Q18" s="45"/>
       <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36" t="s">
+      <c r="S18" s="36" t="s">
         <v>470</v>
       </c>
-      <c r="U18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="32">
+        <v>81.731999999999999</v>
+      </c>
       <c r="V18" s="32">
-        <v>81.731999999999999</v>
+        <v>674</v>
       </c>
       <c r="W18" s="32">
-        <v>674</v>
+        <v>1777</v>
       </c>
       <c r="X18" s="32">
-        <v>1777</v>
-      </c>
-      <c r="Y18" s="32">
         <v>70.230999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="36" t="s">
         <v>471</v>
       </c>
@@ -10894,25 +10874,24 @@
       </c>
       <c r="Q19" s="45"/>
       <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="36" t="s">
+      <c r="S19" s="36" t="s">
         <v>472</v>
       </c>
-      <c r="U19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="32">
+        <v>7.5119999999999996</v>
+      </c>
       <c r="V19" s="32">
-        <v>7.5119999999999996</v>
+        <v>444</v>
       </c>
       <c r="W19" s="32">
-        <v>444</v>
+        <v>1590</v>
       </c>
       <c r="X19" s="32">
-        <v>1590</v>
-      </c>
-      <c r="Y19" s="32">
         <v>17.052</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
         <v>473</v>
       </c>
@@ -10963,25 +10942,24 @@
       <c r="R20" s="36" t="s">
         <v>474</v>
       </c>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36" t="s">
+      <c r="S20" s="36" t="s">
         <v>475</v>
       </c>
-      <c r="U20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="32">
+        <v>177.47900000000001</v>
+      </c>
       <c r="V20" s="32">
-        <v>177.47900000000001</v>
+        <v>310</v>
       </c>
       <c r="W20" s="32">
-        <v>310</v>
+        <v>1439</v>
       </c>
       <c r="X20" s="32">
-        <v>1439</v>
-      </c>
-      <c r="Y20" s="32">
         <v>17.135999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="s">
         <v>476</v>
       </c>
@@ -11030,25 +11008,24 @@
       </c>
       <c r="Q21" s="45"/>
       <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36" t="s">
+      <c r="S21" s="36" t="s">
         <v>477</v>
       </c>
-      <c r="U21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="32">
+        <v>148.428</v>
+      </c>
       <c r="V21" s="32">
-        <v>148.428</v>
+        <v>176</v>
       </c>
       <c r="W21" s="32">
-        <v>176</v>
+        <v>262</v>
       </c>
       <c r="X21" s="32">
-        <v>262</v>
-      </c>
-      <c r="Y21" s="32">
         <v>148.35900000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>478</v>
       </c>
@@ -11095,25 +11072,24 @@
       </c>
       <c r="Q22" s="45"/>
       <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36" t="s">
+      <c r="S22" s="36" t="s">
         <v>479</v>
       </c>
-      <c r="U22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="32">
+        <v>58.637999999999998</v>
+      </c>
       <c r="V22" s="32">
-        <v>58.637999999999998</v>
+        <v>600</v>
       </c>
       <c r="W22" s="32">
-        <v>600</v>
+        <v>1554</v>
       </c>
       <c r="X22" s="32">
-        <v>1554</v>
-      </c>
-      <c r="Y22" s="32">
         <v>32.293999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
         <v>480</v>
       </c>
@@ -11164,25 +11140,24 @@
       <c r="R23" s="36" t="s">
         <v>482</v>
       </c>
-      <c r="S23" s="36"/>
-      <c r="T23" s="36" t="s">
+      <c r="S23" s="36" t="s">
         <v>483</v>
       </c>
-      <c r="U23" s="31"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="32">
+        <v>1.4279999999999999</v>
+      </c>
       <c r="V23" s="32">
-        <v>1.4279999999999999</v>
+        <v>586</v>
       </c>
       <c r="W23" s="32">
-        <v>586</v>
+        <v>937</v>
       </c>
       <c r="X23" s="32">
-        <v>937</v>
-      </c>
-      <c r="Y23" s="32">
         <v>4.9059999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
         <v>484</v>
       </c>
@@ -11231,25 +11206,24 @@
       </c>
       <c r="Q24" s="45"/>
       <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="36" t="s">
+      <c r="S24" s="36" t="s">
         <v>485</v>
       </c>
-      <c r="U24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="32">
+        <v>153.941</v>
+      </c>
       <c r="V24" s="32">
-        <v>153.941</v>
+        <v>358</v>
       </c>
       <c r="W24" s="32">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="X24" s="32">
-        <v>338</v>
-      </c>
-      <c r="Y24" s="32">
         <v>145.24100000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="36" t="s">
         <v>486</v>
       </c>
@@ -11296,25 +11270,24 @@
       <c r="R25" s="36" t="s">
         <v>487</v>
       </c>
-      <c r="S25" s="36"/>
-      <c r="T25" s="36" t="s">
+      <c r="S25" s="36" t="s">
         <v>488</v>
       </c>
-      <c r="U25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="32">
+        <v>11.497</v>
+      </c>
       <c r="V25" s="32">
-        <v>11.497</v>
+        <v>361</v>
       </c>
       <c r="W25" s="32">
-        <v>361</v>
+        <v>602</v>
       </c>
       <c r="X25" s="32">
-        <v>602</v>
-      </c>
-      <c r="Y25" s="32">
         <v>161.066</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="36" t="s">
         <v>489</v>
       </c>
@@ -11363,25 +11336,24 @@
       </c>
       <c r="Q26" s="45"/>
       <c r="R26" s="31"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="36" t="s">
+      <c r="S26" s="36" t="s">
         <v>490</v>
       </c>
-      <c r="U26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="32">
+        <v>146.40899999999999</v>
+      </c>
       <c r="V26" s="32">
-        <v>146.40899999999999</v>
+        <v>439</v>
       </c>
       <c r="W26" s="32">
-        <v>439</v>
+        <v>179</v>
       </c>
       <c r="X26" s="32">
-        <v>179</v>
-      </c>
-      <c r="Y26" s="32">
         <v>140.74700000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="36" t="s">
         <v>491</v>
       </c>
@@ -11432,25 +11404,24 @@
       <c r="R27" s="36" t="s">
         <v>492</v>
       </c>
-      <c r="S27" s="36"/>
-      <c r="T27" s="36" t="s">
+      <c r="S27" s="36" t="s">
         <v>493</v>
       </c>
-      <c r="U27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="32">
+        <v>158.48099999999999</v>
+      </c>
       <c r="V27" s="32">
-        <v>158.48099999999999</v>
+        <v>840</v>
       </c>
       <c r="W27" s="32">
-        <v>840</v>
+        <v>193</v>
       </c>
       <c r="X27" s="32">
-        <v>193</v>
-      </c>
-      <c r="Y27" s="32">
         <v>137.38900000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="36" t="s">
         <v>494</v>
       </c>
@@ -11497,25 +11468,24 @@
       </c>
       <c r="Q28" s="45"/>
       <c r="R28" s="31"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="36" t="s">
+      <c r="S28" s="36" t="s">
         <v>495</v>
       </c>
-      <c r="U28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="32">
+        <v>62.83</v>
+      </c>
       <c r="V28" s="32">
-        <v>62.83</v>
+        <v>803</v>
       </c>
       <c r="W28" s="32">
-        <v>803</v>
+        <v>1584</v>
       </c>
       <c r="X28" s="32">
-        <v>1584</v>
-      </c>
-      <c r="Y28" s="32">
         <v>40.767000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="36" t="s">
         <v>496</v>
       </c>
@@ -11562,25 +11532,24 @@
       </c>
       <c r="Q29" s="45"/>
       <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="T29" s="36" t="s">
+      <c r="S29" s="36" t="s">
         <v>497</v>
       </c>
-      <c r="U29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="32">
+        <v>20.954999999999998</v>
+      </c>
       <c r="V29" s="32">
-        <v>20.954999999999998</v>
+        <v>280</v>
       </c>
       <c r="W29" s="32">
-        <v>280</v>
+        <v>1505</v>
       </c>
       <c r="X29" s="32">
-        <v>1505</v>
-      </c>
-      <c r="Y29" s="32">
         <v>37.334000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="36" t="s">
         <v>498</v>
       </c>
@@ -11625,25 +11594,24 @@
       <c r="P30" s="44"/>
       <c r="Q30" s="45"/>
       <c r="R30" s="31"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="36" t="s">
+      <c r="S30" s="36" t="s">
         <v>499</v>
       </c>
-      <c r="U30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="32">
+        <v>179.17500000000001</v>
+      </c>
       <c r="V30" s="32">
-        <v>179.17500000000001</v>
+        <v>554</v>
       </c>
       <c r="W30" s="32">
-        <v>554</v>
+        <v>1373</v>
       </c>
       <c r="X30" s="32">
-        <v>1373</v>
-      </c>
-      <c r="Y30" s="32">
         <v>36.161000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="36" t="s">
         <v>500</v>
       </c>
@@ -11692,25 +11660,24 @@
       <c r="R31" s="36" t="s">
         <v>501</v>
       </c>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36" t="s">
+      <c r="S31" s="36" t="s">
         <v>502</v>
       </c>
-      <c r="U31" s="31"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="32">
+        <v>179.90299999999999</v>
+      </c>
       <c r="V31" s="32">
-        <v>179.90299999999999</v>
+        <v>450</v>
       </c>
       <c r="W31" s="32">
-        <v>450</v>
+        <v>1166</v>
       </c>
       <c r="X31" s="32">
-        <v>1166</v>
-      </c>
-      <c r="Y31" s="32">
         <v>7.9130000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="36" t="s">
         <v>503</v>
       </c>
@@ -11759,25 +11726,24 @@
       </c>
       <c r="Q32" s="45"/>
       <c r="R32" s="31"/>
-      <c r="S32" s="31"/>
-      <c r="T32" s="36" t="s">
+      <c r="S32" s="36" t="s">
         <v>504</v>
       </c>
-      <c r="U32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="32">
+        <v>177.82499999999999</v>
+      </c>
       <c r="V32" s="32">
-        <v>177.82499999999999</v>
+        <v>346</v>
       </c>
       <c r="W32" s="32">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="X32" s="32">
-        <v>331</v>
-      </c>
-      <c r="Y32" s="32">
         <v>151.66300000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="36" t="s">
         <v>505</v>
       </c>
@@ -11826,25 +11792,24 @@
       </c>
       <c r="Q33" s="45"/>
       <c r="R33" s="36"/>
-      <c r="S33" s="36"/>
-      <c r="T33" s="36" t="s">
+      <c r="S33" s="36" t="s">
         <v>506</v>
       </c>
-      <c r="U33" s="31"/>
+      <c r="T33" s="31"/>
+      <c r="U33" s="32">
+        <v>32.423999999999999</v>
+      </c>
       <c r="V33" s="32">
-        <v>32.423999999999999</v>
+        <v>413</v>
       </c>
       <c r="W33" s="32">
-        <v>413</v>
+        <v>1230</v>
       </c>
       <c r="X33" s="32">
-        <v>1230</v>
-      </c>
-      <c r="Y33" s="32">
         <v>10.1</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="36" t="s">
         <v>507</v>
       </c>
@@ -11893,25 +11858,24 @@
       </c>
       <c r="Q34" s="45"/>
       <c r="R34" s="31"/>
-      <c r="S34" s="31"/>
-      <c r="T34" s="36" t="s">
+      <c r="S34" s="36" t="s">
         <v>508</v>
       </c>
-      <c r="U34" s="31"/>
+      <c r="T34" s="31"/>
+      <c r="U34" s="32">
+        <v>150.50200000000001</v>
+      </c>
       <c r="V34" s="32">
-        <v>150.50200000000001</v>
+        <v>243</v>
       </c>
       <c r="W34" s="32">
-        <v>243</v>
+        <v>501</v>
       </c>
       <c r="X34" s="32">
-        <v>501</v>
-      </c>
-      <c r="Y34" s="32">
         <v>157.625</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="36" t="s">
         <v>509</v>
       </c>
@@ -11962,25 +11926,24 @@
       <c r="R35" s="36" t="s">
         <v>511</v>
       </c>
-      <c r="S35" s="36"/>
-      <c r="T35" s="36" t="s">
+      <c r="S35" s="36" t="s">
         <v>512</v>
       </c>
-      <c r="U35" s="31"/>
+      <c r="T35" s="31"/>
+      <c r="U35" s="32">
+        <v>176.459</v>
+      </c>
       <c r="V35" s="32">
-        <v>176.459</v>
+        <v>384</v>
       </c>
       <c r="W35" s="32">
-        <v>384</v>
+        <v>1094</v>
       </c>
       <c r="X35" s="32">
-        <v>1094</v>
-      </c>
-      <c r="Y35" s="32">
         <v>5.665</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
         <v>513</v>
       </c>
@@ -12029,25 +11992,24 @@
       </c>
       <c r="Q36" s="45"/>
       <c r="R36" s="31"/>
-      <c r="S36" s="31"/>
-      <c r="T36" s="36" t="s">
+      <c r="S36" s="36" t="s">
         <v>514</v>
       </c>
-      <c r="U36" s="31"/>
+      <c r="T36" s="31"/>
+      <c r="U36" s="32">
+        <v>8.4420000000000002</v>
+      </c>
       <c r="V36" s="32">
-        <v>8.4420000000000002</v>
+        <v>472</v>
       </c>
       <c r="W36" s="32">
-        <v>472</v>
+        <v>1043</v>
       </c>
       <c r="X36" s="32">
-        <v>1043</v>
-      </c>
-      <c r="Y36" s="32">
         <v>175.351</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="36" t="s">
         <v>515</v>
       </c>
@@ -12096,25 +12058,24 @@
       </c>
       <c r="Q37" s="45"/>
       <c r="R37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="T37" s="36" t="s">
+      <c r="S37" s="36" t="s">
         <v>517</v>
       </c>
-      <c r="U37" s="31"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="32">
+        <v>165.25700000000001</v>
+      </c>
       <c r="V37" s="32">
-        <v>165.25700000000001</v>
+        <v>294</v>
       </c>
       <c r="W37" s="32">
-        <v>294</v>
+        <v>859</v>
       </c>
       <c r="X37" s="32">
-        <v>859</v>
-      </c>
-      <c r="Y37" s="32">
         <v>167.196</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="36" t="s">
         <v>518</v>
       </c>
@@ -12165,25 +12126,24 @@
       <c r="R38" s="31" t="s">
         <v>519</v>
       </c>
-      <c r="S38" s="31"/>
-      <c r="T38" s="36" t="s">
+      <c r="S38" s="36" t="s">
         <v>520</v>
       </c>
-      <c r="U38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="32">
+        <v>11.696999999999999</v>
+      </c>
       <c r="V38" s="32">
-        <v>11.696999999999999</v>
+        <v>457</v>
       </c>
       <c r="W38" s="32">
-        <v>457</v>
+        <v>1103</v>
       </c>
       <c r="X38" s="32">
-        <v>1103</v>
-      </c>
-      <c r="Y38" s="32">
         <v>8.843</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="36" t="s">
         <v>521</v>
       </c>
@@ -12234,25 +12194,24 @@
       <c r="R39" s="36" t="s">
         <v>522</v>
       </c>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36" t="s">
+      <c r="S39" s="36" t="s">
         <v>523</v>
       </c>
-      <c r="U39" s="31"/>
+      <c r="T39" s="31"/>
+      <c r="U39" s="32">
+        <v>29.138999999999999</v>
+      </c>
       <c r="V39" s="32">
-        <v>29.138999999999999</v>
+        <v>334</v>
       </c>
       <c r="W39" s="32">
-        <v>334</v>
+        <v>1411</v>
       </c>
       <c r="X39" s="32">
-        <v>1411</v>
-      </c>
-      <c r="Y39" s="32">
         <v>12.074</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="36" t="s">
         <v>524</v>
       </c>
@@ -12303,25 +12262,24 @@
       <c r="R40" s="36" t="s">
         <v>525</v>
       </c>
-      <c r="S40" s="36"/>
-      <c r="T40" s="36" t="s">
+      <c r="S40" s="36" t="s">
         <v>526</v>
       </c>
-      <c r="U40" s="31"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="32">
+        <v>28.643000000000001</v>
+      </c>
       <c r="V40" s="32">
-        <v>28.643000000000001</v>
+        <v>348</v>
       </c>
       <c r="W40" s="32">
-        <v>348</v>
+        <v>1391</v>
       </c>
       <c r="X40" s="32">
-        <v>1391</v>
-      </c>
-      <c r="Y40" s="32">
         <v>29.690999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="36" t="s">
         <v>527</v>
       </c>
@@ -12370,25 +12328,24 @@
       </c>
       <c r="Q41" s="45"/>
       <c r="R41" s="36"/>
-      <c r="S41" s="36"/>
-      <c r="T41" s="36" t="s">
+      <c r="S41" s="36" t="s">
         <v>528</v>
       </c>
-      <c r="U41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="32">
+        <v>0.69499999999999995</v>
+      </c>
       <c r="V41" s="32">
-        <v>0.69499999999999995</v>
+        <v>316</v>
       </c>
       <c r="W41" s="32">
-        <v>316</v>
+        <v>1478</v>
       </c>
       <c r="X41" s="32">
-        <v>1478</v>
-      </c>
-      <c r="Y41" s="32">
         <v>43.674999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="36" t="s">
         <v>529</v>
       </c>
@@ -12437,25 +12394,24 @@
       </c>
       <c r="Q42" s="45"/>
       <c r="R42" s="31"/>
-      <c r="S42" s="31"/>
-      <c r="T42" s="36" t="s">
+      <c r="S42" s="36" t="s">
         <v>530</v>
       </c>
-      <c r="U42" s="31"/>
+      <c r="T42" s="31"/>
+      <c r="U42" s="32">
+        <v>178.58099999999999</v>
+      </c>
       <c r="V42" s="32">
-        <v>178.58099999999999</v>
+        <v>217</v>
       </c>
       <c r="W42" s="32">
-        <v>217</v>
+        <v>612</v>
       </c>
       <c r="X42" s="32">
-        <v>612</v>
-      </c>
-      <c r="Y42" s="32">
         <v>166.41900000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="36" t="s">
         <v>531</v>
       </c>
@@ -12506,25 +12462,24 @@
       <c r="R43" s="36" t="s">
         <v>435</v>
       </c>
-      <c r="S43" s="36"/>
-      <c r="T43" s="36" t="s">
+      <c r="S43" s="36" t="s">
         <v>532</v>
       </c>
-      <c r="U43" s="31"/>
+      <c r="T43" s="31"/>
+      <c r="U43" s="32">
+        <v>148.214</v>
+      </c>
       <c r="V43" s="32">
-        <v>148.214</v>
+        <v>762</v>
       </c>
       <c r="W43" s="32">
-        <v>762</v>
+        <v>616</v>
       </c>
       <c r="X43" s="32">
-        <v>616</v>
-      </c>
-      <c r="Y43" s="32">
         <v>143.744</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="36" t="s">
         <v>533</v>
       </c>
@@ -12573,25 +12528,24 @@
       </c>
       <c r="Q44" s="45"/>
       <c r="R44" s="31"/>
-      <c r="S44" s="31"/>
-      <c r="T44" s="36" t="s">
+      <c r="S44" s="36" t="s">
         <v>534</v>
       </c>
-      <c r="U44" s="31"/>
+      <c r="T44" s="31"/>
+      <c r="U44" s="32">
+        <v>7.3410000000000002</v>
+      </c>
       <c r="V44" s="32">
-        <v>7.3410000000000002</v>
+        <v>315</v>
       </c>
       <c r="W44" s="32">
-        <v>315</v>
+        <v>928</v>
       </c>
       <c r="X44" s="32">
-        <v>928</v>
-      </c>
-      <c r="Y44" s="32">
         <v>172.46</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="36" t="s">
         <v>535</v>
       </c>
@@ -12642,25 +12596,24 @@
       <c r="R45" s="36" t="s">
         <v>522</v>
       </c>
-      <c r="S45" s="36"/>
-      <c r="T45" s="36" t="s">
+      <c r="S45" s="36" t="s">
         <v>536</v>
       </c>
-      <c r="U45" s="31"/>
+      <c r="T45" s="31"/>
+      <c r="U45" s="32">
+        <v>151.989</v>
+      </c>
       <c r="V45" s="32">
-        <v>151.989</v>
+        <v>523</v>
       </c>
       <c r="W45" s="32">
-        <v>523</v>
+        <v>371</v>
       </c>
       <c r="X45" s="32">
-        <v>371</v>
-      </c>
-      <c r="Y45" s="32">
         <v>144.82300000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="36" t="s">
         <v>537</v>
       </c>
@@ -12709,25 +12662,24 @@
       </c>
       <c r="Q46" s="45"/>
       <c r="R46" s="31"/>
-      <c r="S46" s="31"/>
-      <c r="T46" s="36" t="s">
+      <c r="S46" s="36" t="s">
         <v>538</v>
       </c>
-      <c r="U46" s="31"/>
+      <c r="T46" s="31"/>
+      <c r="U46" s="32">
+        <v>170.65299999999999</v>
+      </c>
       <c r="V46" s="32">
-        <v>170.65299999999999</v>
+        <v>323</v>
       </c>
       <c r="W46" s="32">
-        <v>323</v>
+        <v>803</v>
       </c>
       <c r="X46" s="32">
-        <v>803</v>
-      </c>
-      <c r="Y46" s="32">
         <v>6.2350000000000003</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="36" t="s">
         <v>539</v>
       </c>
@@ -12776,25 +12728,24 @@
       </c>
       <c r="Q47" s="45"/>
       <c r="R47" s="36"/>
-      <c r="S47" s="36"/>
-      <c r="T47" s="36" t="s">
+      <c r="S47" s="36" t="s">
         <v>540</v>
       </c>
-      <c r="U47" s="31"/>
+      <c r="T47" s="31"/>
+      <c r="U47" s="32">
+        <v>179.50899999999999</v>
+      </c>
       <c r="V47" s="32">
-        <v>179.50899999999999</v>
+        <v>260</v>
       </c>
       <c r="W47" s="32">
-        <v>260</v>
+        <v>957</v>
       </c>
       <c r="X47" s="32">
-        <v>957</v>
-      </c>
-      <c r="Y47" s="32">
         <v>0.6</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="36" t="s">
         <v>541</v>
       </c>
@@ -12843,25 +12794,24 @@
       </c>
       <c r="Q48" s="45"/>
       <c r="R48" s="31"/>
-      <c r="S48" s="31"/>
-      <c r="T48" s="36" t="s">
+      <c r="S48" s="36" t="s">
         <v>542</v>
       </c>
-      <c r="U48" s="31"/>
+      <c r="T48" s="31"/>
+      <c r="U48" s="32">
+        <v>169.089</v>
+      </c>
       <c r="V48" s="32">
-        <v>169.089</v>
+        <v>250</v>
       </c>
       <c r="W48" s="32">
-        <v>250</v>
+        <v>437</v>
       </c>
       <c r="X48" s="32">
-        <v>437</v>
-      </c>
-      <c r="Y48" s="32">
         <v>158.78</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="36" t="s">
         <v>543</v>
       </c>
@@ -12912,25 +12862,24 @@
       <c r="R49" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="S49" s="36"/>
-      <c r="T49" s="36" t="s">
+      <c r="S49" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="U49" s="31"/>
+      <c r="T49" s="31"/>
+      <c r="U49" s="32">
+        <v>1.744</v>
+      </c>
       <c r="V49" s="32">
-        <v>1.744</v>
+        <v>256</v>
       </c>
       <c r="W49" s="32">
-        <v>256</v>
+        <v>986</v>
       </c>
       <c r="X49" s="32">
-        <v>986</v>
-      </c>
-      <c r="Y49" s="32">
         <v>0.82399999999999995</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="36" t="s">
         <v>546</v>
       </c>
@@ -12979,25 +12928,24 @@
       </c>
       <c r="Q50" s="45"/>
       <c r="R50" s="31"/>
-      <c r="S50" s="31"/>
-      <c r="T50" s="36" t="s">
+      <c r="S50" s="36" t="s">
         <v>547</v>
       </c>
-      <c r="U50" s="31"/>
+      <c r="T50" s="31"/>
+      <c r="U50" s="32">
+        <v>175.32599999999999</v>
+      </c>
       <c r="V50" s="32">
-        <v>175.32599999999999</v>
+        <v>389</v>
       </c>
       <c r="W50" s="32">
-        <v>389</v>
+        <v>793</v>
       </c>
       <c r="X50" s="32">
-        <v>793</v>
-      </c>
-      <c r="Y50" s="32">
         <v>166.702</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" s="36" t="s">
         <v>548</v>
       </c>
@@ -13048,25 +12996,24 @@
       <c r="R51" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="S51" s="36"/>
-      <c r="T51" s="36" t="s">
+      <c r="S51" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="U51" s="31"/>
+      <c r="T51" s="31"/>
+      <c r="U51" s="32">
+        <v>136.91800000000001</v>
+      </c>
       <c r="V51" s="32">
-        <v>136.91800000000001</v>
+        <v>690</v>
       </c>
       <c r="W51" s="32">
-        <v>690</v>
+        <v>361</v>
       </c>
       <c r="X51" s="32">
-        <v>361</v>
-      </c>
-      <c r="Y51" s="32">
         <v>137.25399999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="36" t="s">
         <v>551</v>
       </c>
@@ -13117,25 +13064,24 @@
       <c r="R52" s="31" t="s">
         <v>552</v>
       </c>
-      <c r="S52" s="31"/>
-      <c r="T52" s="36" t="s">
+      <c r="S52" s="36" t="s">
         <v>553</v>
       </c>
-      <c r="U52" s="31"/>
+      <c r="T52" s="31"/>
+      <c r="U52" s="32">
+        <v>162.82300000000001</v>
+      </c>
       <c r="V52" s="32">
-        <v>162.82300000000001</v>
+        <v>560</v>
       </c>
       <c r="W52" s="32">
-        <v>560</v>
+        <v>434</v>
       </c>
       <c r="X52" s="32">
-        <v>434</v>
-      </c>
-      <c r="Y52" s="32">
         <v>140.99299999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="36" t="s">
         <v>554</v>
       </c>
@@ -13186,25 +13132,24 @@
       <c r="R53" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="S53" s="36"/>
-      <c r="T53" s="36" t="s">
+      <c r="S53" s="36" t="s">
         <v>556</v>
       </c>
-      <c r="U53" s="31"/>
+      <c r="T53" s="31"/>
+      <c r="U53" s="32">
+        <v>178.18700000000001</v>
+      </c>
       <c r="V53" s="32">
-        <v>178.18700000000001</v>
+        <v>126</v>
       </c>
       <c r="W53" s="32">
-        <v>126</v>
+        <v>885</v>
       </c>
       <c r="X53" s="32">
-        <v>885</v>
-      </c>
-      <c r="Y53" s="32">
         <v>169.45099999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="36" t="s">
         <v>557</v>
       </c>
@@ -13255,25 +13200,24 @@
       <c r="R54" s="31" t="s">
         <v>558</v>
       </c>
-      <c r="S54" s="31"/>
-      <c r="T54" s="36" t="s">
+      <c r="S54" s="36" t="s">
         <v>559</v>
       </c>
-      <c r="U54" s="31"/>
+      <c r="T54" s="31"/>
+      <c r="U54" s="32">
+        <v>177.65</v>
+      </c>
       <c r="V54" s="32">
-        <v>177.65</v>
+        <v>231</v>
       </c>
       <c r="W54" s="32">
-        <v>231</v>
+        <v>492</v>
       </c>
       <c r="X54" s="32">
-        <v>492</v>
-      </c>
-      <c r="Y54" s="32">
         <v>160.91300000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="36" t="s">
         <v>560</v>
       </c>
@@ -13324,25 +13268,24 @@
       <c r="R55" s="36" t="s">
         <v>561</v>
       </c>
-      <c r="S55" s="36"/>
-      <c r="T55" s="36" t="s">
+      <c r="S55" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="U55" s="31"/>
+      <c r="T55" s="31"/>
+      <c r="U55" s="32">
+        <v>162.65199999999999</v>
+      </c>
       <c r="V55" s="32">
-        <v>162.65199999999999</v>
+        <v>534</v>
       </c>
       <c r="W55" s="32">
-        <v>534</v>
+        <v>334</v>
       </c>
       <c r="X55" s="32">
-        <v>334</v>
-      </c>
-      <c r="Y55" s="32">
         <v>148.047</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" s="36" t="s">
         <v>563</v>
       </c>
@@ -13393,25 +13336,24 @@
       <c r="R56" s="36" t="s">
         <v>564</v>
       </c>
-      <c r="S56" s="36"/>
-      <c r="T56" s="36" t="s">
+      <c r="S56" s="36" t="s">
         <v>565</v>
       </c>
-      <c r="U56" s="31"/>
+      <c r="T56" s="31"/>
+      <c r="U56" s="32">
+        <v>173.017</v>
+      </c>
       <c r="V56" s="32">
-        <v>173.017</v>
+        <v>623</v>
       </c>
       <c r="W56" s="32">
-        <v>623</v>
+        <v>780</v>
       </c>
       <c r="X56" s="32">
-        <v>780</v>
-      </c>
-      <c r="Y56" s="32">
         <v>168.94200000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="36" t="s">
         <v>566</v>
       </c>
@@ -13462,25 +13404,24 @@
       <c r="R57" s="36" t="s">
         <v>567</v>
       </c>
-      <c r="S57" s="36"/>
-      <c r="T57" s="36" t="s">
+      <c r="S57" s="36" t="s">
         <v>568</v>
       </c>
-      <c r="U57" s="31"/>
+      <c r="T57" s="31"/>
+      <c r="U57" s="32">
+        <v>2.6949999999999998</v>
+      </c>
       <c r="V57" s="32">
-        <v>2.6949999999999998</v>
+        <v>365</v>
       </c>
       <c r="W57" s="32">
-        <v>365</v>
+        <v>901</v>
       </c>
       <c r="X57" s="32">
-        <v>901</v>
-      </c>
-      <c r="Y57" s="32">
         <v>10.363</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="36" t="s">
         <v>569</v>
       </c>
@@ -13531,25 +13472,24 @@
       <c r="R58" s="36" t="s">
         <v>570</v>
       </c>
-      <c r="S58" s="36"/>
-      <c r="T58" s="36" t="s">
+      <c r="S58" s="36" t="s">
         <v>571</v>
       </c>
-      <c r="U58" s="31"/>
+      <c r="T58" s="31"/>
+      <c r="U58" s="32">
+        <v>142.97900000000001</v>
+      </c>
       <c r="V58" s="32">
-        <v>142.97900000000001</v>
+        <v>505</v>
       </c>
       <c r="W58" s="32">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="X58" s="32">
-        <v>496</v>
-      </c>
-      <c r="Y58" s="32">
         <v>137.89699999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" s="36" t="s">
         <v>572</v>
       </c>
@@ -13600,25 +13540,24 @@
       <c r="R59" s="36" t="s">
         <v>570</v>
       </c>
-      <c r="S59" s="36"/>
-      <c r="T59" s="36" t="s">
+      <c r="S59" s="36" t="s">
         <v>573</v>
       </c>
-      <c r="U59" s="31"/>
+      <c r="T59" s="31"/>
+      <c r="U59" s="32">
+        <v>4.375</v>
+      </c>
       <c r="V59" s="32">
-        <v>4.375</v>
+        <v>539</v>
       </c>
       <c r="W59" s="32">
-        <v>539</v>
+        <v>1326</v>
       </c>
       <c r="X59" s="32">
-        <v>1326</v>
-      </c>
-      <c r="Y59" s="32">
         <v>21.132000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60" s="36" t="s">
         <v>574</v>
       </c>
@@ -13667,25 +13606,24 @@
       </c>
       <c r="Q60" s="45"/>
       <c r="R60" s="31"/>
-      <c r="S60" s="31"/>
-      <c r="T60" s="36" t="s">
+      <c r="S60" s="36" t="s">
         <v>575</v>
       </c>
-      <c r="U60" s="31"/>
+      <c r="T60" s="31"/>
+      <c r="U60" s="32">
+        <v>168.053</v>
+      </c>
       <c r="V60" s="32">
-        <v>168.053</v>
+        <v>237</v>
       </c>
       <c r="W60" s="32">
-        <v>237</v>
+        <v>1410</v>
       </c>
       <c r="X60" s="32">
-        <v>1410</v>
-      </c>
-      <c r="Y60" s="32">
         <v>179.52600000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" s="36" t="s">
         <v>576</v>
       </c>
@@ -13736,25 +13674,24 @@
       <c r="R61" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="S61" s="36"/>
-      <c r="T61" s="36" t="s">
+      <c r="S61" s="36" t="s">
         <v>578</v>
       </c>
-      <c r="U61" s="31"/>
+      <c r="T61" s="31"/>
+      <c r="U61" s="32">
+        <v>177.34100000000001</v>
+      </c>
       <c r="V61" s="32">
-        <v>177.34100000000001</v>
+        <v>314</v>
       </c>
       <c r="W61" s="32">
-        <v>314</v>
+        <v>607</v>
       </c>
       <c r="X61" s="32">
-        <v>607</v>
-      </c>
-      <c r="Y61" s="32">
         <v>175.77799999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="36" t="s">
         <v>579</v>
       </c>
@@ -13803,25 +13740,24 @@
       </c>
       <c r="Q62" s="45"/>
       <c r="R62" s="31"/>
-      <c r="S62" s="31"/>
-      <c r="T62" s="36" t="s">
+      <c r="S62" s="36" t="s">
         <v>580</v>
       </c>
-      <c r="U62" s="31"/>
+      <c r="T62" s="31"/>
+      <c r="U62" s="32">
+        <v>177.245</v>
+      </c>
       <c r="V62" s="32">
-        <v>177.245</v>
+        <v>251</v>
       </c>
       <c r="W62" s="32">
-        <v>251</v>
+        <v>1369</v>
       </c>
       <c r="X62" s="32">
-        <v>1369</v>
-      </c>
-      <c r="Y62" s="32">
         <v>16.236999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="36" t="s">
         <v>581</v>
       </c>
@@ -13870,25 +13806,24 @@
       </c>
       <c r="Q63" s="45"/>
       <c r="R63" s="36"/>
-      <c r="S63" s="36"/>
-      <c r="T63" s="36" t="s">
+      <c r="S63" s="36" t="s">
         <v>582</v>
       </c>
-      <c r="U63" s="31"/>
+      <c r="T63" s="31"/>
+      <c r="U63" s="32">
+        <v>179.649</v>
+      </c>
       <c r="V63" s="32">
-        <v>179.649</v>
+        <v>554</v>
       </c>
       <c r="W63" s="32">
-        <v>554</v>
+        <v>1187</v>
       </c>
       <c r="X63" s="32">
-        <v>1187</v>
-      </c>
-      <c r="Y63" s="32">
         <v>17.719000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64" s="36" t="s">
         <v>583</v>
       </c>
@@ -13939,25 +13874,24 @@
       <c r="R64" s="31" t="s">
         <v>584</v>
       </c>
-      <c r="S64" s="31"/>
-      <c r="T64" s="36" t="s">
+      <c r="S64" s="36" t="s">
         <v>585</v>
       </c>
-      <c r="U64" s="31"/>
+      <c r="T64" s="31"/>
+      <c r="U64" s="32">
+        <v>179.62100000000001</v>
+      </c>
       <c r="V64" s="32">
-        <v>179.62100000000001</v>
+        <v>156</v>
       </c>
       <c r="W64" s="32">
-        <v>156</v>
+        <v>1066</v>
       </c>
       <c r="X64" s="32">
-        <v>1066</v>
-      </c>
-      <c r="Y64" s="32">
         <v>5.9089999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65" s="36" t="s">
         <v>586</v>
       </c>
@@ -14006,25 +13940,24 @@
       </c>
       <c r="Q65" s="45"/>
       <c r="R65" s="36"/>
-      <c r="S65" s="36"/>
-      <c r="T65" s="36" t="s">
+      <c r="S65" s="36" t="s">
         <v>587</v>
       </c>
-      <c r="U65" s="31"/>
+      <c r="T65" s="31"/>
+      <c r="U65" s="32">
+        <v>174.197</v>
+      </c>
       <c r="V65" s="32">
-        <v>174.197</v>
+        <v>860</v>
       </c>
       <c r="W65" s="32">
-        <v>860</v>
+        <v>302</v>
       </c>
       <c r="X65" s="32">
-        <v>302</v>
-      </c>
-      <c r="Y65" s="32">
         <v>132.65700000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66" s="36" t="s">
         <v>588</v>
       </c>
@@ -14073,25 +14006,24 @@
       </c>
       <c r="Q66" s="45"/>
       <c r="R66" s="31"/>
-      <c r="S66" s="31"/>
-      <c r="T66" s="36" t="s">
+      <c r="S66" s="36" t="s">
         <v>589</v>
       </c>
-      <c r="U66" s="31"/>
+      <c r="T66" s="31"/>
+      <c r="U66" s="32">
+        <v>25.257999999999999</v>
+      </c>
       <c r="V66" s="32">
-        <v>25.257999999999999</v>
+        <v>272</v>
       </c>
       <c r="W66" s="32">
-        <v>272</v>
+        <v>1493</v>
       </c>
       <c r="X66" s="32">
-        <v>1493</v>
-      </c>
-      <c r="Y66" s="32">
         <v>28.216000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67" s="36" t="s">
         <v>590</v>
       </c>
@@ -14142,25 +14074,24 @@
       </c>
       <c r="Q67" s="45"/>
       <c r="R67" s="36"/>
-      <c r="S67" s="36"/>
-      <c r="T67" s="36" t="s">
+      <c r="S67" s="36" t="s">
         <v>592</v>
       </c>
-      <c r="U67" s="31"/>
+      <c r="T67" s="31"/>
+      <c r="U67" s="33">
+        <v>108.375</v>
+      </c>
       <c r="V67" s="33">
-        <v>108.375</v>
+        <v>0</v>
       </c>
       <c r="W67" s="33">
-        <v>0</v>
+        <v>518</v>
       </c>
       <c r="X67" s="33">
-        <v>518</v>
-      </c>
-      <c r="Y67" s="33">
         <v>151.57</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68" s="36" t="s">
         <v>593</v>
       </c>
@@ -14209,25 +14140,24 @@
       </c>
       <c r="Q68" s="45"/>
       <c r="R68" s="31"/>
-      <c r="S68" s="31"/>
-      <c r="T68" s="36" t="s">
+      <c r="S68" s="36" t="s">
         <v>594</v>
       </c>
-      <c r="U68" s="31"/>
+      <c r="T68" s="31"/>
+      <c r="U68" s="32">
+        <v>2.1669999999999998</v>
+      </c>
       <c r="V68" s="32">
-        <v>2.1669999999999998</v>
+        <v>474</v>
       </c>
       <c r="W68" s="32">
-        <v>474</v>
+        <v>1068</v>
       </c>
       <c r="X68" s="32">
-        <v>1068</v>
-      </c>
-      <c r="Y68" s="32">
         <v>3.8239999999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69" s="36" t="s">
         <v>595</v>
       </c>
@@ -14278,25 +14208,24 @@
       <c r="R69" s="31" t="s">
         <v>596</v>
       </c>
-      <c r="S69" s="31"/>
-      <c r="T69" s="36" t="s">
+      <c r="S69" s="36" t="s">
         <v>597</v>
       </c>
-      <c r="U69" s="31"/>
+      <c r="T69" s="31"/>
+      <c r="U69" s="32">
+        <v>175.417</v>
+      </c>
       <c r="V69" s="32">
-        <v>175.417</v>
+        <v>323</v>
       </c>
       <c r="W69" s="32">
-        <v>323</v>
+        <v>1004</v>
       </c>
       <c r="X69" s="32">
-        <v>1004</v>
-      </c>
-      <c r="Y69" s="32">
         <v>179.72800000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70" s="36" t="s">
         <v>598</v>
       </c>
@@ -14345,25 +14274,24 @@
       </c>
       <c r="Q70" s="45"/>
       <c r="R70" s="36"/>
-      <c r="S70" s="36"/>
-      <c r="T70" s="36" t="s">
+      <c r="S70" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="U70" s="31"/>
+      <c r="T70" s="31"/>
+      <c r="U70" s="32">
+        <v>1.0840000000000001</v>
+      </c>
       <c r="V70" s="32">
-        <v>1.0840000000000001</v>
+        <v>432</v>
       </c>
       <c r="W70" s="32">
-        <v>432</v>
+        <v>1044</v>
       </c>
       <c r="X70" s="32">
-        <v>1044</v>
-      </c>
-      <c r="Y70" s="32">
         <v>7.3040000000000003</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71" s="36" t="s">
         <v>600</v>
       </c>
@@ -14414,25 +14342,24 @@
       <c r="R71" s="36" t="s">
         <v>601</v>
       </c>
-      <c r="S71" s="36"/>
-      <c r="T71" s="36" t="s">
+      <c r="S71" s="36" t="s">
         <v>602</v>
       </c>
-      <c r="U71" s="31"/>
+      <c r="T71" s="31"/>
+      <c r="U71" s="32">
+        <v>0.246</v>
+      </c>
       <c r="V71" s="32">
-        <v>0.246</v>
+        <v>281</v>
       </c>
       <c r="W71" s="32">
-        <v>281</v>
+        <v>1150</v>
       </c>
       <c r="X71" s="32">
-        <v>1150</v>
-      </c>
-      <c r="Y71" s="32">
         <v>10.095000000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72" s="36" t="s">
         <v>603</v>
       </c>
@@ -14481,25 +14408,24 @@
       </c>
       <c r="Q72" s="45"/>
       <c r="R72" s="31"/>
-      <c r="S72" s="31"/>
-      <c r="T72" s="36" t="s">
+      <c r="S72" s="36" t="s">
         <v>604</v>
       </c>
-      <c r="U72" s="31"/>
+      <c r="T72" s="31"/>
+      <c r="U72" s="32">
+        <v>7.6849999999999996</v>
+      </c>
       <c r="V72" s="32">
-        <v>7.6849999999999996</v>
+        <v>664</v>
       </c>
       <c r="W72" s="32">
-        <v>664</v>
+        <v>1631</v>
       </c>
       <c r="X72" s="32">
-        <v>1631</v>
-      </c>
-      <c r="Y72" s="32">
         <v>36.875999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73" s="36" t="s">
         <v>605</v>
       </c>
@@ -14548,25 +14474,24 @@
       </c>
       <c r="Q73" s="45"/>
       <c r="R73" s="36"/>
-      <c r="S73" s="36"/>
-      <c r="T73" s="36" t="s">
+      <c r="S73" s="36" t="s">
         <v>606</v>
       </c>
-      <c r="U73" s="31"/>
+      <c r="T73" s="31"/>
+      <c r="U73" s="32">
+        <v>2.0609999999999999</v>
+      </c>
       <c r="V73" s="32">
-        <v>2.0609999999999999</v>
+        <v>224</v>
       </c>
       <c r="W73" s="32">
-        <v>224</v>
+        <v>1273</v>
       </c>
       <c r="X73" s="32">
-        <v>1273</v>
-      </c>
-      <c r="Y73" s="32">
         <v>11.913</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74" s="36" t="s">
         <v>607</v>
       </c>
@@ -14613,25 +14538,24 @@
       </c>
       <c r="Q74" s="45"/>
       <c r="R74" s="31"/>
-      <c r="S74" s="31"/>
-      <c r="T74" s="36" t="s">
+      <c r="S74" s="36" t="s">
         <v>608</v>
       </c>
-      <c r="U74" s="31"/>
+      <c r="T74" s="31"/>
+      <c r="U74" s="32">
+        <v>177.51499999999999</v>
+      </c>
       <c r="V74" s="32">
-        <v>177.51499999999999</v>
+        <v>231</v>
       </c>
       <c r="W74" s="32">
-        <v>231</v>
+        <v>575</v>
       </c>
       <c r="X74" s="32">
-        <v>575</v>
-      </c>
-      <c r="Y74" s="32">
         <v>160.36199999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75" s="36" t="s">
         <v>609</v>
       </c>
@@ -14678,25 +14602,24 @@
       </c>
       <c r="Q75" s="45"/>
       <c r="R75" s="36"/>
-      <c r="S75" s="36"/>
-      <c r="T75" s="36" t="s">
+      <c r="S75" s="36" t="s">
         <v>610</v>
       </c>
-      <c r="U75" s="31"/>
+      <c r="T75" s="31"/>
+      <c r="U75" s="32">
+        <v>164.85599999999999</v>
+      </c>
       <c r="V75" s="32">
-        <v>164.85599999999999</v>
+        <v>254</v>
       </c>
       <c r="W75" s="32">
-        <v>254</v>
+        <v>403</v>
       </c>
       <c r="X75" s="32">
-        <v>403</v>
-      </c>
-      <c r="Y75" s="32">
         <v>174.143</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76" s="36" t="s">
         <v>611</v>
       </c>
@@ -14741,25 +14664,24 @@
       <c r="P76" s="44"/>
       <c r="Q76" s="45"/>
       <c r="R76" s="31"/>
-      <c r="S76" s="31"/>
-      <c r="T76" s="36" t="s">
+      <c r="S76" s="36" t="s">
         <v>612</v>
       </c>
-      <c r="U76" s="31"/>
+      <c r="T76" s="31"/>
+      <c r="U76" s="32">
+        <v>159.98500000000001</v>
+      </c>
       <c r="V76" s="32">
-        <v>159.98500000000001</v>
+        <v>426</v>
       </c>
       <c r="W76" s="32">
-        <v>426</v>
+        <v>1568</v>
       </c>
       <c r="X76" s="32">
-        <v>1568</v>
-      </c>
-      <c r="Y76" s="32">
         <v>1.831</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77" s="36" t="s">
         <v>613</v>
       </c>
@@ -14808,25 +14730,24 @@
       </c>
       <c r="Q77" s="45"/>
       <c r="R77" s="36"/>
-      <c r="S77" s="36"/>
-      <c r="T77" s="36" t="s">
+      <c r="S77" s="36" t="s">
         <v>614</v>
       </c>
-      <c r="U77" s="31"/>
+      <c r="T77" s="31"/>
+      <c r="U77" s="32">
+        <v>0.78200000000000003</v>
+      </c>
       <c r="V77" s="32">
-        <v>0.78200000000000003</v>
+        <v>252</v>
       </c>
       <c r="W77" s="32">
-        <v>252</v>
+        <v>989</v>
       </c>
       <c r="X77" s="32">
-        <v>989</v>
-      </c>
-      <c r="Y77" s="32">
         <v>179.096</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78" s="36" t="s">
         <v>615</v>
       </c>
@@ -14871,25 +14792,24 @@
       <c r="P78" s="44"/>
       <c r="Q78" s="45"/>
       <c r="R78" s="31"/>
-      <c r="S78" s="31"/>
-      <c r="T78" s="36" t="s">
+      <c r="S78" s="36" t="s">
         <v>616</v>
       </c>
-      <c r="U78" s="31"/>
+      <c r="T78" s="31"/>
+      <c r="U78" s="32">
+        <v>2.6669999999999998</v>
+      </c>
       <c r="V78" s="32">
-        <v>2.6669999999999998</v>
+        <v>342</v>
       </c>
       <c r="W78" s="32">
-        <v>342</v>
+        <v>774</v>
       </c>
       <c r="X78" s="32">
-        <v>774</v>
-      </c>
-      <c r="Y78" s="32">
         <v>157.55799999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79" s="36" t="s">
         <v>617</v>
       </c>
@@ -14928,25 +14848,24 @@
       <c r="P79" s="44"/>
       <c r="Q79" s="45"/>
       <c r="R79" s="36"/>
-      <c r="S79" s="36"/>
-      <c r="T79" s="36" t="s">
+      <c r="S79" s="36" t="s">
         <v>618</v>
       </c>
-      <c r="U79" s="31"/>
+      <c r="T79" s="31"/>
+      <c r="U79" s="32">
+        <v>173.66300000000001</v>
+      </c>
       <c r="V79" s="32">
-        <v>173.66300000000001</v>
+        <v>328</v>
       </c>
       <c r="W79" s="32">
-        <v>328</v>
+        <v>632</v>
       </c>
       <c r="X79" s="32">
-        <v>632</v>
-      </c>
-      <c r="Y79" s="32">
         <v>168.54499999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80" s="36" t="s">
         <v>619</v>
       </c>
@@ -14985,25 +14904,24 @@
       <c r="P80" s="44"/>
       <c r="Q80" s="45"/>
       <c r="R80" s="31"/>
-      <c r="S80" s="31"/>
-      <c r="T80" s="36" t="s">
+      <c r="S80" s="36" t="s">
         <v>620</v>
       </c>
-      <c r="U80" s="31"/>
+      <c r="T80" s="31"/>
+      <c r="U80" s="32">
+        <v>5.1630000000000003</v>
+      </c>
       <c r="V80" s="32">
-        <v>5.1630000000000003</v>
+        <v>506</v>
       </c>
       <c r="W80" s="32">
-        <v>506</v>
+        <v>1269</v>
       </c>
       <c r="X80" s="32">
-        <v>1269</v>
-      </c>
-      <c r="Y80" s="32">
         <v>23.709</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81" s="36" t="s">
         <v>621</v>
       </c>
@@ -15042,25 +14960,24 @@
       <c r="P81" s="44"/>
       <c r="Q81" s="45"/>
       <c r="R81" s="36"/>
-      <c r="S81" s="36"/>
-      <c r="T81" s="36" t="s">
+      <c r="S81" s="36" t="s">
         <v>622</v>
       </c>
-      <c r="U81" s="31"/>
+      <c r="T81" s="31"/>
+      <c r="U81" s="32">
+        <v>170.92500000000001</v>
+      </c>
       <c r="V81" s="32">
-        <v>170.92500000000001</v>
+        <v>337</v>
       </c>
       <c r="W81" s="32">
-        <v>337</v>
+        <v>805</v>
       </c>
       <c r="X81" s="32">
-        <v>805</v>
-      </c>
-      <c r="Y81" s="32">
         <v>164.971</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82" s="36" t="s">
         <v>623</v>
       </c>
@@ -15099,25 +15016,24 @@
       <c r="P82" s="44"/>
       <c r="Q82" s="45"/>
       <c r="R82" s="31"/>
-      <c r="S82" s="31"/>
-      <c r="T82" s="36" t="s">
+      <c r="S82" s="36" t="s">
         <v>624</v>
       </c>
-      <c r="U82" s="31"/>
+      <c r="T82" s="31"/>
+      <c r="U82" s="32">
+        <v>13.935</v>
+      </c>
       <c r="V82" s="32">
-        <v>13.935</v>
+        <v>834</v>
       </c>
       <c r="W82" s="32">
-        <v>834</v>
+        <v>1477</v>
       </c>
       <c r="X82" s="32">
-        <v>1477</v>
-      </c>
-      <c r="Y82" s="32">
         <v>39.302</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A83" s="36" t="s">
         <v>625</v>
       </c>
@@ -15156,25 +15072,24 @@
       <c r="P83" s="44"/>
       <c r="Q83" s="45"/>
       <c r="R83" s="36"/>
-      <c r="S83" s="36"/>
-      <c r="T83" s="36" t="s">
+      <c r="S83" s="36" t="s">
         <v>626</v>
       </c>
-      <c r="U83" s="31"/>
+      <c r="T83" s="31"/>
+      <c r="U83" s="32">
+        <v>7.7489999999999997</v>
+      </c>
       <c r="V83" s="32">
-        <v>7.7489999999999997</v>
+        <v>798</v>
       </c>
       <c r="W83" s="32">
-        <v>798</v>
+        <v>1733</v>
       </c>
       <c r="X83" s="32">
-        <v>1733</v>
-      </c>
-      <c r="Y83" s="32">
         <v>42.851999999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A84" s="36" t="s">
         <v>627</v>
       </c>
@@ -15213,25 +15128,24 @@
       <c r="P84" s="44"/>
       <c r="Q84" s="45"/>
       <c r="R84" s="31"/>
-      <c r="S84" s="31"/>
-      <c r="T84" s="36" t="s">
+      <c r="S84" s="36" t="s">
         <v>628</v>
       </c>
-      <c r="U84" s="31"/>
+      <c r="T84" s="31"/>
+      <c r="U84" s="32">
+        <v>150.15</v>
+      </c>
       <c r="V84" s="32">
-        <v>150.15</v>
+        <v>500</v>
       </c>
       <c r="W84" s="32">
-        <v>500</v>
+        <v>446</v>
       </c>
       <c r="X84" s="32">
-        <v>446</v>
-      </c>
-      <c r="Y84" s="32">
         <v>148.51400000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A85" s="36" t="s">
         <v>629</v>
       </c>
@@ -15270,25 +15184,24 @@
       <c r="P85" s="44"/>
       <c r="Q85" s="45"/>
       <c r="R85" s="36"/>
-      <c r="S85" s="36"/>
-      <c r="T85" s="36" t="s">
+      <c r="S85" s="36" t="s">
         <v>630</v>
       </c>
-      <c r="U85" s="31"/>
+      <c r="T85" s="31"/>
+      <c r="U85" s="32">
+        <v>19.245000000000001</v>
+      </c>
       <c r="V85" s="32">
-        <v>19.245000000000001</v>
+        <v>352</v>
       </c>
       <c r="W85" s="32">
-        <v>352</v>
+        <v>1443</v>
       </c>
       <c r="X85" s="32">
-        <v>1443</v>
-      </c>
-      <c r="Y85" s="32">
         <v>27.349</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A86" s="36" t="s">
         <v>631</v>
       </c>
@@ -15327,25 +15240,24 @@
       <c r="P86" s="44"/>
       <c r="Q86" s="45"/>
       <c r="R86" s="31"/>
-      <c r="S86" s="31"/>
-      <c r="T86" s="36" t="s">
+      <c r="S86" s="36" t="s">
         <v>632</v>
       </c>
-      <c r="U86" s="31"/>
+      <c r="T86" s="31"/>
+      <c r="U86" s="32">
+        <v>11.449</v>
+      </c>
       <c r="V86" s="32">
-        <v>11.449</v>
+        <v>196</v>
       </c>
       <c r="W86" s="32">
-        <v>196</v>
+        <v>1472</v>
       </c>
       <c r="X86" s="32">
-        <v>1472</v>
-      </c>
-      <c r="Y86" s="32">
         <v>25.879000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A87" s="36" t="s">
         <v>633</v>
       </c>
@@ -15384,25 +15296,24 @@
       <c r="P87" s="44"/>
       <c r="Q87" s="45"/>
       <c r="R87" s="36"/>
-      <c r="S87" s="36"/>
-      <c r="T87" s="36" t="s">
+      <c r="S87" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="U87" s="31"/>
+      <c r="T87" s="31"/>
+      <c r="U87" s="32">
+        <v>172.89400000000001</v>
+      </c>
       <c r="V87" s="32">
-        <v>172.89400000000001</v>
+        <v>527</v>
       </c>
       <c r="W87" s="32">
-        <v>527</v>
+        <v>841</v>
       </c>
       <c r="X87" s="32">
-        <v>841</v>
-      </c>
-      <c r="Y87" s="32">
         <v>168.78700000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A88" s="36" t="s">
         <v>635</v>
       </c>
@@ -15441,25 +15352,24 @@
       <c r="P88" s="44"/>
       <c r="Q88" s="45"/>
       <c r="R88" s="31"/>
-      <c r="S88" s="31"/>
-      <c r="T88" s="36" t="s">
+      <c r="S88" s="36" t="s">
         <v>636</v>
       </c>
-      <c r="U88" s="31"/>
+      <c r="T88" s="31"/>
+      <c r="U88" s="32">
+        <v>176.66900000000001</v>
+      </c>
       <c r="V88" s="32">
-        <v>176.66900000000001</v>
+        <v>408</v>
       </c>
       <c r="W88" s="32">
-        <v>408</v>
+        <v>1164</v>
       </c>
       <c r="X88" s="32">
-        <v>1164</v>
-      </c>
-      <c r="Y88" s="32">
         <v>6.4820000000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A89" s="36" t="s">
         <v>637</v>
       </c>
@@ -15498,25 +15408,24 @@
       <c r="P89" s="44"/>
       <c r="Q89" s="45"/>
       <c r="R89" s="36"/>
-      <c r="S89" s="36"/>
-      <c r="T89" s="36" t="s">
+      <c r="S89" s="36" t="s">
         <v>638</v>
       </c>
-      <c r="U89" s="31"/>
+      <c r="T89" s="31"/>
+      <c r="U89" s="32">
+        <v>175.965</v>
+      </c>
       <c r="V89" s="32">
-        <v>175.965</v>
+        <v>649</v>
       </c>
       <c r="W89" s="32">
-        <v>649</v>
+        <v>187</v>
       </c>
       <c r="X89" s="32">
-        <v>187</v>
-      </c>
-      <c r="Y89" s="32">
         <v>133.16300000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A90" s="36" t="s">
         <v>639</v>
       </c>
@@ -15555,25 +15464,24 @@
       <c r="P90" s="44"/>
       <c r="Q90" s="45"/>
       <c r="R90" s="31"/>
-      <c r="S90" s="31"/>
-      <c r="T90" s="36" t="s">
+      <c r="S90" s="36" t="s">
         <v>640</v>
       </c>
-      <c r="U90" s="31"/>
+      <c r="T90" s="31"/>
+      <c r="U90" s="32">
+        <v>154.78399999999999</v>
+      </c>
       <c r="V90" s="32">
-        <v>154.78399999999999</v>
+        <v>618</v>
       </c>
       <c r="W90" s="32">
-        <v>618</v>
+        <v>816</v>
       </c>
       <c r="X90" s="32">
-        <v>816</v>
-      </c>
-      <c r="Y90" s="32">
         <v>171.33699999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A91" s="36" t="s">
         <v>641</v>
       </c>
@@ -15612,25 +15520,24 @@
       <c r="P91" s="44"/>
       <c r="Q91" s="45"/>
       <c r="R91" s="36"/>
-      <c r="S91" s="36"/>
-      <c r="T91" s="36" t="s">
+      <c r="S91" s="36" t="s">
         <v>642</v>
       </c>
-      <c r="U91" s="31"/>
+      <c r="T91" s="31"/>
+      <c r="U91" s="32">
+        <v>11.927</v>
+      </c>
       <c r="V91" s="32">
-        <v>11.927</v>
+        <v>291</v>
       </c>
       <c r="W91" s="32">
-        <v>291</v>
+        <v>1551</v>
       </c>
       <c r="X91" s="32">
-        <v>1551</v>
-      </c>
-      <c r="Y91" s="32">
         <v>37.087000000000003</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A92" s="36" t="s">
         <v>643</v>
       </c>
@@ -15669,25 +15576,24 @@
       <c r="P92" s="44"/>
       <c r="Q92" s="45"/>
       <c r="R92" s="31"/>
-      <c r="S92" s="31"/>
-      <c r="T92" s="36" t="s">
+      <c r="S92" s="36" t="s">
         <v>644</v>
       </c>
-      <c r="U92" s="31"/>
+      <c r="T92" s="31"/>
+      <c r="U92" s="32">
+        <v>176.43799999999999</v>
+      </c>
       <c r="V92" s="32">
-        <v>176.43799999999999</v>
+        <v>351</v>
       </c>
       <c r="W92" s="32">
-        <v>351</v>
+        <v>1029</v>
       </c>
       <c r="X92" s="32">
-        <v>1029</v>
-      </c>
-      <c r="Y92" s="32">
         <v>1.3220000000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A93" s="36" t="s">
         <v>645</v>
       </c>
@@ -15726,25 +15632,24 @@
       <c r="P93" s="44"/>
       <c r="Q93" s="45"/>
       <c r="R93" s="36"/>
-      <c r="S93" s="36"/>
-      <c r="T93" s="36" t="s">
+      <c r="S93" s="36" t="s">
         <v>646</v>
       </c>
-      <c r="U93" s="31"/>
+      <c r="T93" s="31"/>
+      <c r="U93" s="32">
+        <v>11.6</v>
+      </c>
       <c r="V93" s="32">
-        <v>11.6</v>
+        <v>308</v>
       </c>
       <c r="W93" s="32">
-        <v>308</v>
+        <v>1074</v>
       </c>
       <c r="X93" s="32">
-        <v>1074</v>
-      </c>
-      <c r="Y93" s="32">
         <v>10.319000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A94" s="36" t="s">
         <v>647</v>
       </c>
@@ -15783,25 +15688,24 @@
       <c r="P94" s="44"/>
       <c r="Q94" s="45"/>
       <c r="R94" s="31"/>
-      <c r="S94" s="31"/>
-      <c r="T94" s="36" t="s">
+      <c r="S94" s="36" t="s">
         <v>648</v>
       </c>
-      <c r="U94" s="31"/>
+      <c r="T94" s="31"/>
+      <c r="U94" s="32">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="V94" s="32">
-        <v>1.4999999999999999E-2</v>
+        <v>296</v>
       </c>
       <c r="W94" s="32">
-        <v>296</v>
+        <v>865</v>
       </c>
       <c r="X94" s="32">
-        <v>865</v>
-      </c>
-      <c r="Y94" s="32">
         <v>178.4</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A95" s="36" t="s">
         <v>649</v>
       </c>
@@ -15840,25 +15744,24 @@
       <c r="P95" s="44"/>
       <c r="Q95" s="45"/>
       <c r="R95" s="36"/>
-      <c r="S95" s="36"/>
-      <c r="T95" s="36" t="s">
+      <c r="S95" s="36" t="s">
         <v>650</v>
       </c>
-      <c r="U95" s="31"/>
+      <c r="T95" s="31"/>
+      <c r="U95" s="32">
+        <v>179.495</v>
+      </c>
       <c r="V95" s="32">
-        <v>179.495</v>
+        <v>462</v>
       </c>
       <c r="W95" s="32">
-        <v>462</v>
+        <v>941</v>
       </c>
       <c r="X95" s="32">
-        <v>941</v>
-      </c>
-      <c r="Y95" s="32">
         <v>4.4429999999999996</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A96" s="36" t="s">
         <v>651</v>
       </c>
@@ -15897,25 +15800,24 @@
       <c r="P96" s="44"/>
       <c r="Q96" s="45"/>
       <c r="R96" s="31"/>
-      <c r="S96" s="31"/>
-      <c r="T96" s="36" t="s">
+      <c r="S96" s="36" t="s">
         <v>652</v>
       </c>
-      <c r="U96" s="31"/>
+      <c r="T96" s="31"/>
+      <c r="U96" s="32">
+        <v>179.685</v>
+      </c>
       <c r="V96" s="32">
-        <v>179.685</v>
+        <v>396</v>
       </c>
       <c r="W96" s="32">
-        <v>396</v>
+        <v>1053</v>
       </c>
       <c r="X96" s="32">
-        <v>1053</v>
-      </c>
-      <c r="Y96" s="32">
         <v>11.166</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A97" s="36" t="s">
         <v>653</v>
       </c>
@@ -15954,25 +15856,24 @@
       <c r="P97" s="44"/>
       <c r="Q97" s="45"/>
       <c r="R97" s="36"/>
-      <c r="S97" s="36"/>
-      <c r="T97" s="36" t="s">
+      <c r="S97" s="36" t="s">
         <v>654</v>
       </c>
-      <c r="U97" s="31"/>
+      <c r="T97" s="31"/>
+      <c r="U97" s="32">
+        <v>28.321999999999999</v>
+      </c>
       <c r="V97" s="32">
-        <v>28.321999999999999</v>
+        <v>205</v>
       </c>
       <c r="W97" s="32">
-        <v>205</v>
+        <v>1738</v>
       </c>
       <c r="X97" s="32">
-        <v>1738</v>
-      </c>
-      <c r="Y97" s="32">
         <v>42.859000000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A98" s="36" t="s">
         <v>655</v>
       </c>
@@ -16011,25 +15912,24 @@
       <c r="P98" s="44"/>
       <c r="Q98" s="45"/>
       <c r="R98" s="31"/>
-      <c r="S98" s="31"/>
-      <c r="T98" s="36" t="s">
+      <c r="S98" s="36" t="s">
         <v>656</v>
       </c>
-      <c r="U98" s="31"/>
+      <c r="T98" s="31"/>
+      <c r="U98" s="32">
+        <v>4.4020000000000001</v>
+      </c>
       <c r="V98" s="32">
-        <v>4.4020000000000001</v>
+        <v>621</v>
       </c>
       <c r="W98" s="32">
-        <v>621</v>
+        <v>1582</v>
       </c>
       <c r="X98" s="32">
-        <v>1582</v>
-      </c>
-      <c r="Y98" s="32">
         <v>42.378999999999998</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A99" s="36" t="s">
         <v>657</v>
       </c>
@@ -16068,25 +15968,24 @@
       <c r="P99" s="44"/>
       <c r="Q99" s="45"/>
       <c r="R99" s="36"/>
-      <c r="S99" s="36"/>
-      <c r="T99" s="36" t="s">
+      <c r="S99" s="36" t="s">
         <v>658</v>
       </c>
-      <c r="U99" s="31"/>
+      <c r="T99" s="31"/>
+      <c r="U99" s="32">
+        <v>7.7350000000000003</v>
+      </c>
       <c r="V99" s="32">
-        <v>7.7350000000000003</v>
+        <v>270</v>
       </c>
       <c r="W99" s="32">
-        <v>270</v>
+        <v>1262</v>
       </c>
       <c r="X99" s="32">
-        <v>1262</v>
-      </c>
-      <c r="Y99" s="32">
         <v>10.645</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A100" s="36" t="s">
         <v>659</v>
       </c>
@@ -16125,25 +16024,24 @@
       <c r="P100" s="44"/>
       <c r="Q100" s="45"/>
       <c r="R100" s="31"/>
-      <c r="S100" s="31"/>
-      <c r="T100" s="36" t="s">
+      <c r="S100" s="36" t="s">
         <v>660</v>
       </c>
-      <c r="U100" s="31"/>
+      <c r="T100" s="31"/>
+      <c r="U100" s="32">
+        <v>8.7469999999999999</v>
+      </c>
       <c r="V100" s="32">
-        <v>8.7469999999999999</v>
+        <v>524</v>
       </c>
       <c r="W100" s="32">
-        <v>524</v>
+        <v>1599</v>
       </c>
       <c r="X100" s="32">
-        <v>1599</v>
-      </c>
-      <c r="Y100" s="32">
         <v>30.655999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A101" s="36" t="s">
         <v>661</v>
       </c>
@@ -16182,25 +16080,24 @@
       <c r="P101" s="44"/>
       <c r="Q101" s="45"/>
       <c r="R101" s="36"/>
-      <c r="S101" s="36"/>
-      <c r="T101" s="36" t="s">
+      <c r="S101" s="36" t="s">
         <v>662</v>
       </c>
-      <c r="U101" s="31"/>
+      <c r="T101" s="31"/>
+      <c r="U101" s="32">
+        <v>177.97399999999999</v>
+      </c>
       <c r="V101" s="32">
-        <v>177.97399999999999</v>
+        <v>412</v>
       </c>
       <c r="W101" s="32">
-        <v>412</v>
+        <v>626</v>
       </c>
       <c r="X101" s="32">
-        <v>626</v>
-      </c>
-      <c r="Y101" s="32">
         <v>151.06700000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A102" s="36" t="s">
         <v>663</v>
       </c>
@@ -16239,25 +16136,24 @@
       <c r="P102" s="44"/>
       <c r="Q102" s="45"/>
       <c r="R102" s="31"/>
-      <c r="S102" s="31"/>
-      <c r="T102" s="36" t="s">
+      <c r="S102" s="36" t="s">
         <v>664</v>
       </c>
-      <c r="U102" s="31"/>
+      <c r="T102" s="31"/>
+      <c r="U102" s="32">
+        <v>1.5269999999999999</v>
+      </c>
       <c r="V102" s="32">
-        <v>1.5269999999999999</v>
+        <v>262</v>
       </c>
       <c r="W102" s="32">
-        <v>262</v>
+        <v>716</v>
       </c>
       <c r="X102" s="32">
-        <v>716</v>
-      </c>
-      <c r="Y102" s="32">
         <v>173.238</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A103" s="36" t="s">
         <v>665</v>
       </c>
@@ -16296,25 +16192,24 @@
       <c r="P103" s="44"/>
       <c r="Q103" s="45"/>
       <c r="R103" s="36"/>
-      <c r="S103" s="36"/>
-      <c r="T103" s="36" t="s">
+      <c r="S103" s="36" t="s">
         <v>666</v>
       </c>
-      <c r="U103" s="31"/>
+      <c r="T103" s="31"/>
+      <c r="U103" s="32">
+        <v>3.2919999999999998</v>
+      </c>
       <c r="V103" s="32">
-        <v>3.2919999999999998</v>
+        <v>402</v>
       </c>
       <c r="W103" s="32">
-        <v>402</v>
+        <v>929</v>
       </c>
       <c r="X103" s="32">
-        <v>929</v>
-      </c>
-      <c r="Y103" s="32">
         <v>4.2450000000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A104" s="36" t="s">
         <v>667</v>
       </c>
@@ -16353,25 +16248,24 @@
       <c r="P104" s="44"/>
       <c r="Q104" s="45"/>
       <c r="R104" s="31"/>
-      <c r="S104" s="31"/>
-      <c r="T104" s="36" t="s">
+      <c r="S104" s="36" t="s">
         <v>668</v>
       </c>
-      <c r="U104" s="31"/>
+      <c r="T104" s="31"/>
+      <c r="U104" s="32">
+        <v>29.491</v>
+      </c>
       <c r="V104" s="32">
-        <v>29.491</v>
+        <v>562</v>
       </c>
       <c r="W104" s="32">
-        <v>562</v>
+        <v>1539</v>
       </c>
       <c r="X104" s="32">
-        <v>1539</v>
-      </c>
-      <c r="Y104" s="32">
         <v>46.417999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A105" s="36" t="s">
         <v>669</v>
       </c>
@@ -16410,25 +16304,24 @@
       <c r="P105" s="44"/>
       <c r="Q105" s="45"/>
       <c r="R105" s="36"/>
-      <c r="S105" s="36"/>
-      <c r="T105" s="36" t="s">
+      <c r="S105" s="36" t="s">
         <v>670</v>
       </c>
-      <c r="U105" s="31"/>
+      <c r="T105" s="31"/>
+      <c r="U105" s="32">
+        <v>6.476</v>
+      </c>
       <c r="V105" s="32">
-        <v>6.476</v>
+        <v>427</v>
       </c>
       <c r="W105" s="32">
-        <v>427</v>
+        <v>1064</v>
       </c>
       <c r="X105" s="32">
-        <v>1064</v>
-      </c>
-      <c r="Y105" s="32">
         <v>8.5039999999999996</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A106" s="36" t="s">
         <v>671</v>
       </c>
@@ -16469,25 +16362,24 @@
       <c r="P106" s="44"/>
       <c r="Q106" s="45"/>
       <c r="R106" s="31"/>
-      <c r="S106" s="31"/>
-      <c r="T106" s="36" t="s">
+      <c r="S106" s="36" t="s">
         <v>673</v>
       </c>
-      <c r="U106" s="31"/>
+      <c r="T106" s="31"/>
+      <c r="U106" s="32">
+        <v>26.748000000000001</v>
+      </c>
       <c r="V106" s="32">
-        <v>26.748000000000001</v>
+        <v>958</v>
       </c>
       <c r="W106" s="32">
-        <v>958</v>
+        <v>1558</v>
       </c>
       <c r="X106" s="32">
-        <v>1558</v>
-      </c>
-      <c r="Y106" s="32">
         <v>49.359000000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A107" s="36" t="s">
         <v>674</v>
       </c>
@@ -16528,25 +16420,24 @@
       <c r="P107" s="44"/>
       <c r="Q107" s="45"/>
       <c r="R107" s="36"/>
-      <c r="S107" s="36"/>
-      <c r="T107" s="36" t="s">
+      <c r="S107" s="36" t="s">
         <v>676</v>
       </c>
-      <c r="U107" s="31"/>
+      <c r="T107" s="31"/>
+      <c r="U107" s="33">
+        <v>69.34</v>
+      </c>
       <c r="V107" s="33">
-        <v>69.34</v>
+        <v>2046</v>
       </c>
       <c r="W107" s="33">
-        <v>2046</v>
+        <v>1560</v>
       </c>
       <c r="X107" s="33">
-        <v>1560</v>
-      </c>
-      <c r="Y107" s="33">
         <v>66.331000000000003</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A108" s="36" t="s">
         <v>677</v>
       </c>
@@ -16585,25 +16476,24 @@
       <c r="P108" s="44"/>
       <c r="Q108" s="45"/>
       <c r="R108" s="31"/>
-      <c r="S108" s="31"/>
-      <c r="T108" s="36" t="s">
+      <c r="S108" s="36" t="s">
         <v>678</v>
       </c>
-      <c r="U108" s="31"/>
+      <c r="T108" s="31"/>
+      <c r="U108" s="32">
+        <v>179.541</v>
+      </c>
       <c r="V108" s="32">
-        <v>179.541</v>
+        <v>189</v>
       </c>
       <c r="W108" s="32">
-        <v>189</v>
+        <v>962</v>
       </c>
       <c r="X108" s="32">
-        <v>962</v>
-      </c>
-      <c r="Y108" s="32">
         <v>2.5680000000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A109" s="36" t="s">
         <v>679</v>
       </c>
@@ -16642,25 +16532,24 @@
       <c r="P109" s="44"/>
       <c r="Q109" s="45"/>
       <c r="R109" s="36"/>
-      <c r="S109" s="36"/>
-      <c r="T109" s="36" t="s">
+      <c r="S109" s="36" t="s">
         <v>680</v>
       </c>
-      <c r="U109" s="31"/>
+      <c r="T109" s="31"/>
+      <c r="U109" s="32">
+        <v>169.05799999999999</v>
+      </c>
       <c r="V109" s="32">
-        <v>169.05799999999999</v>
+        <v>462</v>
       </c>
       <c r="W109" s="32">
-        <v>462</v>
+        <v>1317</v>
       </c>
       <c r="X109" s="32">
-        <v>1317</v>
-      </c>
-      <c r="Y109" s="32">
         <v>12.132</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A110" s="36" t="s">
         <v>681</v>
       </c>
@@ -16699,25 +16588,24 @@
       <c r="P110" s="44"/>
       <c r="Q110" s="45"/>
       <c r="R110" s="31"/>
-      <c r="S110" s="31"/>
-      <c r="T110" s="36" t="s">
+      <c r="S110" s="36" t="s">
         <v>682</v>
       </c>
-      <c r="U110" s="31"/>
+      <c r="T110" s="31"/>
+      <c r="U110" s="32">
+        <v>9.4329999999999998</v>
+      </c>
       <c r="V110" s="32">
-        <v>9.4329999999999998</v>
+        <v>488</v>
       </c>
       <c r="W110" s="32">
-        <v>488</v>
+        <v>1124</v>
       </c>
       <c r="X110" s="32">
-        <v>1124</v>
-      </c>
-      <c r="Y110" s="32">
         <v>19.934999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A111" s="36" t="s">
         <v>683</v>
       </c>
@@ -16756,25 +16644,24 @@
       <c r="P111" s="44"/>
       <c r="Q111" s="45"/>
       <c r="R111" s="36"/>
-      <c r="S111" s="36"/>
-      <c r="T111" s="36" t="s">
+      <c r="S111" s="36" t="s">
         <v>684</v>
       </c>
-      <c r="U111" s="31"/>
+      <c r="T111" s="31"/>
+      <c r="U111" s="32">
+        <v>13.023</v>
+      </c>
       <c r="V111" s="32">
-        <v>13.023</v>
+        <v>396</v>
       </c>
       <c r="W111" s="32">
-        <v>396</v>
+        <v>1070</v>
       </c>
       <c r="X111" s="32">
-        <v>1070</v>
-      </c>
-      <c r="Y111" s="32">
         <v>12.315</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A112" s="36" t="s">
         <v>685</v>
       </c>
@@ -16813,25 +16700,24 @@
       <c r="P112" s="44"/>
       <c r="Q112" s="45"/>
       <c r="R112" s="31"/>
-      <c r="S112" s="31"/>
-      <c r="T112" s="36" t="s">
+      <c r="S112" s="36" t="s">
         <v>686</v>
       </c>
-      <c r="U112" s="31"/>
+      <c r="T112" s="31"/>
+      <c r="U112" s="32">
+        <v>158.49799999999999</v>
+      </c>
       <c r="V112" s="32">
-        <v>158.49799999999999</v>
+        <v>735</v>
       </c>
       <c r="W112" s="32">
-        <v>735</v>
+        <v>338</v>
       </c>
       <c r="X112" s="32">
-        <v>338</v>
-      </c>
-      <c r="Y112" s="32">
         <v>143.62200000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A113" s="36" t="s">
         <v>687</v>
       </c>
@@ -16870,25 +16756,24 @@
       <c r="P113" s="44"/>
       <c r="Q113" s="45"/>
       <c r="R113" s="36"/>
-      <c r="S113" s="36"/>
-      <c r="T113" s="36" t="s">
+      <c r="S113" s="36" t="s">
         <v>688</v>
       </c>
-      <c r="U113" s="31"/>
+      <c r="T113" s="31"/>
+      <c r="U113" s="32">
+        <v>177.11</v>
+      </c>
       <c r="V113" s="32">
-        <v>177.11</v>
+        <v>264</v>
       </c>
       <c r="W113" s="32">
-        <v>264</v>
+        <v>814</v>
       </c>
       <c r="X113" s="32">
-        <v>814</v>
-      </c>
-      <c r="Y113" s="32">
         <v>165.15899999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A114" s="36" t="s">
         <v>689</v>
       </c>
@@ -16927,25 +16812,24 @@
       <c r="P114" s="44"/>
       <c r="Q114" s="45"/>
       <c r="R114" s="31"/>
-      <c r="S114" s="31"/>
-      <c r="T114" s="36" t="s">
+      <c r="S114" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="U114" s="31"/>
+      <c r="T114" s="31"/>
+      <c r="U114" s="32">
+        <v>175.69300000000001</v>
+      </c>
       <c r="V114" s="32">
-        <v>175.69300000000001</v>
+        <v>388</v>
       </c>
       <c r="W114" s="32">
-        <v>388</v>
+        <v>974</v>
       </c>
       <c r="X114" s="32">
-        <v>974</v>
-      </c>
-      <c r="Y114" s="32">
         <v>173.71299999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A115" s="36" t="s">
         <v>691</v>
       </c>
@@ -16984,25 +16868,24 @@
       <c r="P115" s="44"/>
       <c r="Q115" s="45"/>
       <c r="R115" s="36"/>
-      <c r="S115" s="36"/>
-      <c r="T115" s="36" t="s">
+      <c r="S115" s="36" t="s">
         <v>692</v>
       </c>
-      <c r="U115" s="31"/>
+      <c r="T115" s="31"/>
+      <c r="U115" s="32">
+        <v>4.4999999999999998E-2</v>
+      </c>
       <c r="V115" s="32">
-        <v>4.4999999999999998E-2</v>
+        <v>277</v>
       </c>
       <c r="W115" s="32">
-        <v>277</v>
+        <v>1027</v>
       </c>
       <c r="X115" s="32">
-        <v>1027</v>
-      </c>
-      <c r="Y115" s="32">
         <v>2.782</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A116" s="36" t="s">
         <v>693</v>
       </c>
@@ -17041,25 +16924,24 @@
       <c r="P116" s="44"/>
       <c r="Q116" s="45"/>
       <c r="R116" s="31"/>
-      <c r="S116" s="31"/>
-      <c r="T116" s="36" t="s">
+      <c r="S116" s="36" t="s">
         <v>694</v>
       </c>
-      <c r="U116" s="31"/>
+      <c r="T116" s="31"/>
+      <c r="U116" s="32">
+        <v>4.1349999999999998</v>
+      </c>
       <c r="V116" s="32">
-        <v>4.1349999999999998</v>
+        <v>275</v>
       </c>
       <c r="W116" s="32">
-        <v>275</v>
+        <v>1132</v>
       </c>
       <c r="X116" s="32">
-        <v>1132</v>
-      </c>
-      <c r="Y116" s="32">
         <v>13.478999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A117" s="36" t="s">
         <v>695</v>
       </c>
@@ -17098,25 +16980,24 @@
       <c r="P117" s="44"/>
       <c r="Q117" s="45"/>
       <c r="R117" s="36"/>
-      <c r="S117" s="36"/>
-      <c r="T117" s="36" t="s">
+      <c r="S117" s="36" t="s">
         <v>696</v>
       </c>
-      <c r="U117" s="31"/>
+      <c r="T117" s="31"/>
+      <c r="U117" s="33">
+        <v>56.332999999999998</v>
+      </c>
       <c r="V117" s="33">
-        <v>56.332999999999998</v>
+        <v>1338</v>
       </c>
       <c r="W117" s="33">
-        <v>1338</v>
+        <v>962</v>
       </c>
       <c r="X117" s="33">
-        <v>962</v>
-      </c>
-      <c r="Y117" s="33">
         <v>126.849</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A118" s="36" t="s">
         <v>697</v>
       </c>
@@ -17157,25 +17038,24 @@
       <c r="P118" s="44"/>
       <c r="Q118" s="45"/>
       <c r="R118" s="31"/>
-      <c r="S118" s="31"/>
-      <c r="T118" s="36" t="s">
+      <c r="S118" s="36" t="s">
         <v>699</v>
       </c>
-      <c r="U118" s="31"/>
+      <c r="T118" s="31"/>
+      <c r="U118" s="32">
+        <v>23.157</v>
+      </c>
       <c r="V118" s="32">
-        <v>23.157</v>
+        <v>171</v>
       </c>
       <c r="W118" s="32">
-        <v>171</v>
+        <v>1064</v>
       </c>
       <c r="X118" s="32">
-        <v>1064</v>
-      </c>
-      <c r="Y118" s="32">
         <v>11.435</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A119" s="36" t="s">
         <v>700</v>
       </c>
@@ -17214,25 +17094,24 @@
       <c r="P119" s="44"/>
       <c r="Q119" s="45"/>
       <c r="R119" s="36"/>
-      <c r="S119" s="36"/>
-      <c r="T119" s="36" t="s">
+      <c r="S119" s="36" t="s">
         <v>701</v>
       </c>
-      <c r="U119" s="31"/>
+      <c r="T119" s="31"/>
+      <c r="U119" s="32">
+        <v>1.423</v>
+      </c>
       <c r="V119" s="32">
-        <v>1.423</v>
+        <v>330</v>
       </c>
       <c r="W119" s="32">
-        <v>330</v>
+        <v>1232</v>
       </c>
       <c r="X119" s="32">
-        <v>1232</v>
-      </c>
-      <c r="Y119" s="32">
         <v>5.2930000000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A120" s="36" t="s">
         <v>702</v>
       </c>
@@ -17271,25 +17150,24 @@
       <c r="P120" s="44"/>
       <c r="Q120" s="45"/>
       <c r="R120" s="31"/>
-      <c r="S120" s="31"/>
-      <c r="T120" s="36" t="s">
+      <c r="S120" s="36" t="s">
         <v>703</v>
       </c>
-      <c r="U120" s="31"/>
+      <c r="T120" s="31"/>
+      <c r="U120" s="32">
+        <v>19.629000000000001</v>
+      </c>
       <c r="V120" s="32">
-        <v>19.629000000000001</v>
+        <v>575</v>
       </c>
       <c r="W120" s="32">
-        <v>575</v>
+        <v>1521</v>
       </c>
       <c r="X120" s="32">
-        <v>1521</v>
-      </c>
-      <c r="Y120" s="32">
         <v>50.594000000000001</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A121" s="36" t="s">
         <v>704</v>
       </c>
@@ -17324,25 +17202,24 @@
       <c r="P121" s="44"/>
       <c r="Q121" s="45"/>
       <c r="R121" s="36"/>
-      <c r="S121" s="36"/>
-      <c r="T121" s="36" t="s">
+      <c r="S121" s="36" t="s">
         <v>705</v>
       </c>
-      <c r="U121" s="31"/>
+      <c r="T121" s="31"/>
+      <c r="U121" s="32">
+        <v>169.715</v>
+      </c>
       <c r="V121" s="32">
-        <v>169.715</v>
+        <v>717</v>
       </c>
       <c r="W121" s="32">
-        <v>717</v>
+        <v>857</v>
       </c>
       <c r="X121" s="32">
-        <v>857</v>
-      </c>
-      <c r="Y121" s="32">
         <v>166.70099999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A122" s="36" t="s">
         <v>706</v>
       </c>
@@ -17377,25 +17254,24 @@
       <c r="P122" s="44"/>
       <c r="Q122" s="45"/>
       <c r="R122" s="31"/>
-      <c r="S122" s="31"/>
-      <c r="T122" s="36" t="s">
+      <c r="S122" s="36" t="s">
         <v>707</v>
       </c>
-      <c r="U122" s="31"/>
+      <c r="T122" s="31"/>
+      <c r="U122" s="32">
+        <v>67.323999999999998</v>
+      </c>
       <c r="V122" s="32">
-        <v>67.323999999999998</v>
+        <v>822</v>
       </c>
       <c r="W122" s="32">
-        <v>822</v>
+        <v>1287</v>
       </c>
       <c r="X122" s="32">
-        <v>1287</v>
-      </c>
-      <c r="Y122" s="32">
         <v>33.662999999999997</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A123" s="36" t="s">
         <v>708</v>
       </c>
@@ -17430,25 +17306,24 @@
       <c r="P123" s="44"/>
       <c r="Q123" s="45"/>
       <c r="R123" s="36"/>
-      <c r="S123" s="36"/>
-      <c r="T123" s="36" t="s">
+      <c r="S123" s="36" t="s">
         <v>709</v>
       </c>
-      <c r="U123" s="31"/>
+      <c r="T123" s="31"/>
+      <c r="U123" s="32">
+        <v>154.31399999999999</v>
+      </c>
       <c r="V123" s="32">
-        <v>154.31399999999999</v>
+        <v>704</v>
       </c>
       <c r="W123" s="32">
-        <v>704</v>
+        <v>628</v>
       </c>
       <c r="X123" s="32">
-        <v>628</v>
-      </c>
-      <c r="Y123" s="32">
         <v>159.42699999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A124" s="36" t="s">
         <v>710</v>
       </c>
@@ -17483,25 +17358,24 @@
       <c r="P124" s="44"/>
       <c r="Q124" s="45"/>
       <c r="R124" s="31"/>
-      <c r="S124" s="31"/>
-      <c r="T124" s="36" t="s">
+      <c r="S124" s="36" t="s">
         <v>711</v>
       </c>
-      <c r="U124" s="31"/>
+      <c r="T124" s="31"/>
+      <c r="U124" s="32">
+        <v>106.84099999999999</v>
+      </c>
       <c r="V124" s="32">
-        <v>106.84099999999999</v>
+        <v>1279</v>
       </c>
       <c r="W124" s="32">
-        <v>1279</v>
+        <v>1529</v>
       </c>
       <c r="X124" s="32">
-        <v>1529</v>
-      </c>
-      <c r="Y124" s="32">
         <v>85.126000000000005</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A125" s="36" t="s">
         <v>712</v>
       </c>
@@ -17536,25 +17410,24 @@
       <c r="P125" s="44"/>
       <c r="Q125" s="45"/>
       <c r="R125" s="36"/>
-      <c r="S125" s="36"/>
-      <c r="T125" s="36" t="s">
+      <c r="S125" s="36" t="s">
         <v>713</v>
       </c>
-      <c r="U125" s="31"/>
+      <c r="T125" s="31"/>
+      <c r="U125" s="32">
+        <v>131.15</v>
+      </c>
       <c r="V125" s="32">
-        <v>131.15</v>
+        <v>1173</v>
       </c>
       <c r="W125" s="32">
-        <v>1173</v>
+        <v>655</v>
       </c>
       <c r="X125" s="32">
-        <v>655</v>
-      </c>
-      <c r="Y125" s="32">
         <v>100.914</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A126" s="36" t="s">
         <v>714</v>
       </c>
@@ -17589,25 +17462,24 @@
       <c r="P126" s="44"/>
       <c r="Q126" s="45"/>
       <c r="R126" s="31"/>
-      <c r="S126" s="31"/>
-      <c r="T126" s="36" t="s">
+      <c r="S126" s="36" t="s">
         <v>715</v>
       </c>
-      <c r="U126" s="31"/>
+      <c r="T126" s="31"/>
+      <c r="U126" s="32">
+        <v>2.9449999999999998</v>
+      </c>
       <c r="V126" s="32">
-        <v>2.9449999999999998</v>
+        <v>863</v>
       </c>
       <c r="W126" s="32">
-        <v>863</v>
+        <v>838</v>
       </c>
       <c r="X126" s="32">
-        <v>838</v>
-      </c>
-      <c r="Y126" s="32">
         <v>162.78399999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A127" s="36" t="s">
         <v>716</v>
       </c>
@@ -17642,25 +17514,24 @@
       <c r="P127" s="44"/>
       <c r="Q127" s="45"/>
       <c r="R127" s="36"/>
-      <c r="S127" s="36"/>
-      <c r="T127" s="36" t="s">
+      <c r="S127" s="36" t="s">
         <v>717</v>
       </c>
-      <c r="U127" s="31"/>
+      <c r="T127" s="31"/>
+      <c r="U127" s="32">
+        <v>67.882999999999996</v>
+      </c>
       <c r="V127" s="32">
-        <v>67.882999999999996</v>
+        <v>1107</v>
       </c>
       <c r="W127" s="32">
-        <v>1107</v>
+        <v>1336</v>
       </c>
       <c r="X127" s="32">
-        <v>1336</v>
-      </c>
-      <c r="Y127" s="32">
         <v>63.606999999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A128" s="36" t="s">
         <v>718</v>
       </c>
@@ -17699,25 +17570,24 @@
       <c r="R128" s="31" t="s">
         <v>720</v>
       </c>
-      <c r="S128" s="31"/>
-      <c r="T128" s="36" t="s">
+      <c r="S128" s="36" t="s">
         <v>721</v>
       </c>
-      <c r="U128" s="31"/>
+      <c r="T128" s="31"/>
+      <c r="U128" s="33">
+        <v>123.907</v>
+      </c>
       <c r="V128" s="33">
-        <v>123.907</v>
+        <v>0</v>
       </c>
       <c r="W128" s="33">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="X128" s="33">
-        <v>28</v>
-      </c>
-      <c r="Y128" s="33">
         <v>128.149</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A129" s="36" t="s">
         <v>722</v>
       </c>
@@ -17760,25 +17630,24 @@
       <c r="R129" s="36" t="s">
         <v>724</v>
       </c>
-      <c r="S129" s="36"/>
-      <c r="T129" s="36" t="s">
+      <c r="S129" s="36" t="s">
         <v>725</v>
       </c>
-      <c r="U129" s="31"/>
+      <c r="T129" s="31"/>
+      <c r="U129" s="33">
+        <v>82.278999999999996</v>
+      </c>
       <c r="V129" s="33">
-        <v>82.278999999999996</v>
+        <v>882</v>
       </c>
       <c r="W129" s="33">
-        <v>882</v>
+        <v>1409</v>
       </c>
       <c r="X129" s="33">
-        <v>1409</v>
-      </c>
-      <c r="Y129" s="33">
         <v>64.915999999999997</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A130" s="36" t="s">
         <v>726</v>
       </c>
@@ -17813,25 +17682,24 @@
       <c r="P130" s="44"/>
       <c r="Q130" s="45"/>
       <c r="R130" s="31"/>
-      <c r="S130" s="31"/>
-      <c r="T130" s="36" t="s">
+      <c r="S130" s="36" t="s">
         <v>727</v>
       </c>
-      <c r="U130" s="31"/>
+      <c r="T130" s="31"/>
+      <c r="U130" s="32">
+        <v>151.86699999999999</v>
+      </c>
       <c r="V130" s="32">
-        <v>151.86699999999999</v>
+        <v>940</v>
       </c>
       <c r="W130" s="32">
-        <v>940</v>
+        <v>782</v>
       </c>
       <c r="X130" s="32">
-        <v>782</v>
-      </c>
-      <c r="Y130" s="32">
         <v>154.43100000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A131" s="36" t="s">
         <v>728</v>
       </c>
@@ -17880,25 +17748,24 @@
       </c>
       <c r="Q131" s="45"/>
       <c r="R131" s="36"/>
-      <c r="S131" s="36"/>
-      <c r="T131" s="36" t="s">
+      <c r="S131" s="36" t="s">
         <v>729</v>
       </c>
-      <c r="U131" s="31"/>
+      <c r="T131" s="31"/>
+      <c r="U131" s="32">
+        <v>5.141</v>
+      </c>
       <c r="V131" s="32">
-        <v>5.141</v>
+        <v>466</v>
       </c>
       <c r="W131" s="32">
-        <v>466</v>
+        <v>1057</v>
       </c>
       <c r="X131" s="32">
-        <v>1057</v>
-      </c>
-      <c r="Y131" s="32">
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A132" s="36" t="s">
         <v>730</v>
       </c>
@@ -17933,25 +17800,24 @@
       <c r="P132" s="44"/>
       <c r="Q132" s="45"/>
       <c r="R132" s="31"/>
-      <c r="S132" s="31"/>
-      <c r="T132" s="36" t="s">
+      <c r="S132" s="36" t="s">
         <v>731</v>
       </c>
-      <c r="U132" s="31"/>
+      <c r="T132" s="31"/>
+      <c r="U132" s="32">
+        <v>176.75200000000001</v>
+      </c>
       <c r="V132" s="32">
-        <v>176.75200000000001</v>
+        <v>638</v>
       </c>
       <c r="W132" s="32">
-        <v>638</v>
+        <v>918</v>
       </c>
       <c r="X132" s="32">
-        <v>918</v>
-      </c>
-      <c r="Y132" s="32">
         <v>171.81899999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A133" s="36" t="s">
         <v>732</v>
       </c>
@@ -17986,25 +17852,24 @@
       <c r="P133" s="44"/>
       <c r="Q133" s="45"/>
       <c r="R133" s="36"/>
-      <c r="S133" s="36"/>
-      <c r="T133" s="36" t="s">
+      <c r="S133" s="36" t="s">
         <v>733</v>
       </c>
-      <c r="U133" s="31"/>
+      <c r="T133" s="31"/>
+      <c r="U133" s="32">
+        <v>0.48799999999999999</v>
+      </c>
       <c r="V133" s="32">
-        <v>0.48799999999999999</v>
+        <v>527</v>
       </c>
       <c r="W133" s="32">
-        <v>527</v>
+        <v>1264</v>
       </c>
       <c r="X133" s="32">
-        <v>1264</v>
-      </c>
-      <c r="Y133" s="32">
         <v>4.1040000000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A134" s="36" t="s">
         <v>734</v>
       </c>
@@ -18039,26 +17904,26 @@
       <c r="P134" s="44"/>
       <c r="Q134" s="45"/>
       <c r="R134" s="31"/>
-      <c r="S134" s="31"/>
-      <c r="T134" s="36" t="s">
+      <c r="S134" s="36" t="s">
         <v>735</v>
       </c>
-      <c r="U134" s="31"/>
+      <c r="T134" s="31"/>
+      <c r="U134" s="32">
+        <v>168.143</v>
+      </c>
       <c r="V134" s="32">
-        <v>168.143</v>
+        <v>573</v>
       </c>
       <c r="W134" s="32">
-        <v>573</v>
+        <v>387</v>
       </c>
       <c r="X134" s="32">
-        <v>387</v>
-      </c>
-      <c r="Y134" s="32">
         <v>147.221</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>